<commit_message>
CIERRE DE  27 dIC-21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rouss\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROUSS\Documents\GitHub\TRABAJO\01 DOCUEMENTOS\CENTRAL  ARCHIVO  2 0 2 1\CENTRAL # 12  DICIEMBRE   2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775E608C-E48E-446E-9D32-F0ED50600008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="0" windowWidth="16605" windowHeight="10920" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="OCTUBRE      2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="REMISIONES  DICIEMBRE  2021   " sheetId="8" r:id="rId6"/>
     <sheet name="Hoja3" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="J23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="J25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -96,12 +95,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="J23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="J25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,12 +153,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>ROUSS</author>
   </authors>
   <commentList>
-    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{B44F866F-6E3D-45D3-8F47-D59E4679E5CF}">
+    <comment ref="J23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{A3E957BC-2972-413F-9A83-8203341F9F02}">
+    <comment ref="J25" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -212,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="222">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -853,16 +852,37 @@
     <t>JAMON-QUESOS-SALCHICA</t>
   </si>
   <si>
-    <t>Vac-sueldo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Transferencia </t>
+  </si>
+  <si>
+    <t>VAC--SUELDO</t>
+  </si>
+  <si>
+    <t>QUESOS-VERDIRA-LONGANIZA-POLLO</t>
+  </si>
+  <si>
+    <t>COBRO CREDITOS MES ANTERIOR</t>
+  </si>
+  <si>
+    <t>EFECITVO X DEPOSITAR</t>
+  </si>
+  <si>
+    <t>QUESOS-PICAÑA-JAMON-POLLO-PAVO</t>
+  </si>
+  <si>
+    <t>SALCHICHAS-SIRLON-POLLO-QUESOS-ROAST-BEEF--LONGANIZA-PAVO</t>
+  </si>
+  <si>
+    <t>POLLO-SALSAS-PAVOS</t>
+  </si>
+  <si>
+    <t>POLLO-QUESOS-LOMO-CHORIZO-PAVO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -872,7 +892,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1260,8 +1280,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1358,8 +1385,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="82">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -2378,12 +2417,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="385">
+  <cellXfs count="395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3037,6 +3132,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="81" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="84" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="85" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="18" borderId="83" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3196,6 +3315,9 @@
     <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3220,20 +3342,17 @@
     <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="44" fontId="2" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3244,11 +3363,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FFCCFF66"/>
       <color rgb="FF6600FF"/>
       <color rgb="FF66FFFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF00FF99"/>
-      <color rgb="FF0000FF"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FF800000"/>
     </mruColors>
@@ -4804,7 +4924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -4836,23 +4956,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="319"/>
-      <c r="C1" s="321" t="s">
+      <c r="B1" s="329"/>
+      <c r="C1" s="331" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="J1" s="322"/>
-      <c r="K1" s="322"/>
-      <c r="L1" s="322"/>
-      <c r="M1" s="322"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="320"/>
+      <c r="B2" s="330"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -4862,17 +4982,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="323" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="324"/>
+      <c r="B3" s="333" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="334"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="325" t="s">
+      <c r="H3" s="335" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="325"/>
+      <c r="I3" s="335"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -4886,14 +5006,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="326" t="s">
+      <c r="E4" s="336" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="327"/>
-      <c r="H4" s="328" t="s">
+      <c r="F4" s="337"/>
+      <c r="H4" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="329"/>
+      <c r="I4" s="339"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -4903,10 +5023,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="335" t="s">
+      <c r="P4" s="345" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="336"/>
+      <c r="Q4" s="346"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -6347,11 +6467,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="337">
+      <c r="M39" s="347">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="339">
+      <c r="N39" s="349">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -6377,8 +6497,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="338"/>
-      <c r="N40" s="340"/>
+      <c r="M40" s="348"/>
+      <c r="N40" s="350"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -6593,29 +6713,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="341" t="s">
+      <c r="H52" s="351" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="342"/>
+      <c r="I52" s="352"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="343">
+      <c r="K52" s="353">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="344"/>
-      <c r="M52" s="345">
+      <c r="L52" s="354"/>
+      <c r="M52" s="355">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="346"/>
+      <c r="N52" s="356"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="347" t="s">
+      <c r="D53" s="357" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="347"/>
+      <c r="E53" s="357"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -6626,22 +6746,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="347" t="s">
+      <c r="D54" s="357" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="347"/>
+      <c r="E54" s="357"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="348" t="s">
+      <c r="I54" s="358" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="349"/>
-      <c r="K54" s="350">
+      <c r="J54" s="359"/>
+      <c r="K54" s="360">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="351"/>
+      <c r="L54" s="361"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6674,11 +6794,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="352">
+      <c r="K56" s="362">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="353"/>
+      <c r="L56" s="363"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -6695,22 +6815,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="330" t="s">
+      <c r="D58" s="340" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="331"/>
+      <c r="E58" s="341"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="332" t="s">
+      <c r="I58" s="342" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="333"/>
-      <c r="K58" s="334">
+      <c r="J58" s="343"/>
+      <c r="K58" s="344">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="334"/>
+      <c r="L58" s="344"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -6883,7 +7003,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF800000"/>
   </sheetPr>
@@ -8214,7 +8334,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="354" t="s">
+      <c r="B41" s="364" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -8246,7 +8366,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="355"/>
+      <c r="B42" s="365"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -9807,7 +9927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -9842,23 +9962,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="319"/>
-      <c r="C1" s="321" t="s">
+      <c r="B1" s="329"/>
+      <c r="C1" s="331" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="J1" s="322"/>
-      <c r="K1" s="322"/>
-      <c r="L1" s="322"/>
-      <c r="M1" s="322"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="320"/>
+      <c r="B2" s="330"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9868,21 +9988,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="323" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="324"/>
+      <c r="B3" s="333" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="334"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="325" t="s">
+      <c r="H3" s="335" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="325"/>
+      <c r="I3" s="335"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="362" t="s">
+      <c r="P3" s="372" t="s">
         <v>6</v>
       </c>
     </row>
@@ -9897,14 +10017,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="326" t="s">
+      <c r="E4" s="336" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="327"/>
-      <c r="H4" s="328" t="s">
+      <c r="F4" s="337"/>
+      <c r="H4" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="329"/>
+      <c r="I4" s="339"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -9914,14 +10034,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="363"/>
+      <c r="P4" s="373"/>
       <c r="Q4" s="288" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="380" t="s">
+      <c r="W4" s="382" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="380"/>
+      <c r="X4" s="382"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -9972,8 +10092,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="380"/>
-      <c r="X5" s="380"/>
+      <c r="W5" s="382"/>
+      <c r="X5" s="382"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10744,7 +10864,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="375">
+      <c r="W19" s="386">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -10796,7 +10916,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="376"/>
+      <c r="W20" s="387"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -10845,8 +10965,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="377"/>
-      <c r="X21" s="377"/>
+      <c r="W21" s="388"/>
+      <c r="X21" s="388"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -10947,8 +11067,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="378"/>
-      <c r="X23" s="378"/>
+      <c r="W23" s="389"/>
+      <c r="X23" s="389"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -11002,8 +11122,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="378"/>
-      <c r="X24" s="378"/>
+      <c r="W24" s="389"/>
+      <c r="X24" s="389"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -11049,8 +11169,8 @@
       <c r="R25" s="287">
         <v>28952</v>
       </c>
-      <c r="W25" s="379"/>
-      <c r="X25" s="379"/>
+      <c r="W25" s="390"/>
+      <c r="X25" s="390"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -11101,8 +11221,8 @@
       <c r="R26" s="287">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="379"/>
-      <c r="X26" s="379"/>
+      <c r="W26" s="390"/>
+      <c r="X26" s="390"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -11150,9 +11270,9 @@
       <c r="R27" s="287">
         <v>14637</v>
       </c>
-      <c r="W27" s="372"/>
-      <c r="X27" s="373"/>
-      <c r="Y27" s="374"/>
+      <c r="W27" s="383"/>
+      <c r="X27" s="384"/>
+      <c r="Y27" s="385"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11202,9 +11322,9 @@
       <c r="R28" s="287">
         <v>0</v>
       </c>
-      <c r="W28" s="373"/>
-      <c r="X28" s="373"/>
-      <c r="Y28" s="374"/>
+      <c r="W28" s="384"/>
+      <c r="X28" s="384"/>
+      <c r="Y28" s="385"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11539,11 +11659,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="364">
+      <c r="M36" s="374">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="366">
+      <c r="N36" s="376">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -11551,7 +11671,7 @@
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="368">
+      <c r="Q36" s="378">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -11586,13 +11706,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="365"/>
-      <c r="N37" s="367"/>
+      <c r="M37" s="375"/>
+      <c r="N37" s="377"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="369"/>
+      <c r="Q37" s="379"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -11882,26 +12002,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="341" t="s">
+      <c r="H52" s="351" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="342"/>
+      <c r="I52" s="352"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="343">
+      <c r="K52" s="353">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="370"/>
+      <c r="L52" s="380"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="347" t="s">
+      <c r="D53" s="357" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="347"/>
+      <c r="E53" s="357"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -11910,29 +12030,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="371" t="s">
+      <c r="D54" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="371"/>
+      <c r="E54" s="381"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="348" t="s">
+      <c r="I54" s="358" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="349"/>
-      <c r="K54" s="350">
+      <c r="J54" s="359"/>
+      <c r="K54" s="360">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="350"/>
-      <c r="M54" s="356" t="s">
+      <c r="L54" s="360"/>
+      <c r="M54" s="366" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="357"/>
-      <c r="O54" s="357"/>
-      <c r="P54" s="357"/>
-      <c r="Q54" s="358"/>
+      <c r="N54" s="367"/>
+      <c r="O54" s="367"/>
+      <c r="P54" s="367"/>
+      <c r="Q54" s="368"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -11946,11 +12066,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="359"/>
-      <c r="N55" s="360"/>
-      <c r="O55" s="360"/>
-      <c r="P55" s="360"/>
-      <c r="Q55" s="361"/>
+      <c r="M55" s="369"/>
+      <c r="N55" s="370"/>
+      <c r="O55" s="370"/>
+      <c r="P55" s="370"/>
+      <c r="Q55" s="371"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -11968,11 +12088,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="352">
+      <c r="K56" s="362">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="353"/>
+      <c r="L56" s="363"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -11989,22 +12109,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="330" t="s">
+      <c r="D58" s="340" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="331"/>
+      <c r="E58" s="341"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="332" t="s">
+      <c r="I58" s="342" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="333"/>
-      <c r="K58" s="334">
+      <c r="J58" s="343"/>
+      <c r="K58" s="344">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="334"/>
+      <c r="L58" s="344"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -12186,7 +12306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
@@ -14575,7 +14695,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="381" t="s">
+      <c r="F87" s="391" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -14588,7 +14708,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="382"/>
+      <c r="F88" s="392"/>
       <c r="K88" s="1"/>
       <c r="L88" s="97"/>
       <c r="M88" s="3"/>
@@ -14892,14 +15012,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF6600FF"/>
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14921,29 +15041,30 @@
     <col min="16" max="16" width="16.85546875" customWidth="1"/>
     <col min="17" max="17" width="18.140625" style="225" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="227" customWidth="1"/>
-    <col min="19" max="21" width="11.42578125" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="1" customWidth="1"/>
     <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="319"/>
-      <c r="C1" s="321" t="s">
+      <c r="B1" s="329"/>
+      <c r="C1" s="331" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
-      <c r="H1" s="322"/>
-      <c r="I1" s="322"/>
-      <c r="J1" s="322"/>
-      <c r="K1" s="322"/>
-      <c r="L1" s="322"/>
-      <c r="M1" s="322"/>
+      <c r="D1" s="332"/>
+      <c r="E1" s="332"/>
+      <c r="F1" s="332"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="332"/>
+      <c r="I1" s="332"/>
+      <c r="J1" s="332"/>
+      <c r="K1" s="332"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="332"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="320"/>
+      <c r="B2" s="330"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -14953,25 +15074,28 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="323" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="324"/>
+      <c r="B3" s="333" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="334"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="325" t="s">
+      <c r="H3" s="335" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="325"/>
+      <c r="I3" s="335"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="362" t="s">
+      <c r="P3" s="372" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R3" s="393" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -14982,14 +15106,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="326" t="s">
+      <c r="E4" s="336" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="327"/>
-      <c r="H4" s="328" t="s">
+      <c r="F4" s="337"/>
+      <c r="H4" s="338" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="329"/>
+      <c r="I4" s="339"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -14999,14 +15123,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="363"/>
-      <c r="Q4" s="288" t="s">
-        <v>209</v>
-      </c>
-      <c r="W4" s="380" t="s">
+      <c r="P4" s="373"/>
+      <c r="Q4" s="326" t="s">
+        <v>217</v>
+      </c>
+      <c r="R4" s="394"/>
+      <c r="W4" s="382" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="380"/>
+      <c r="X4" s="382"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15040,34 +15165,35 @@
         <v>44536</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="L5" s="9">
         <f>1800+857.14</f>
         <v>2657.14</v>
       </c>
       <c r="M5" s="32">
-        <v>1146750</v>
+        <v>0</v>
       </c>
       <c r="N5" s="33">
         <v>36272</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>214</v>
-      </c>
+      <c r="O5" s="322"/>
       <c r="P5" s="34">
         <f>N5+M5+L5+I5+C5</f>
-        <v>1193196.6399999999</v>
-      </c>
-      <c r="Q5" s="289">
+        <v>46446.64</v>
+      </c>
+      <c r="Q5" s="321">
         <f>P5-F5</f>
-        <v>1125195.6399999999</v>
-      </c>
-      <c r="R5" s="229">
-        <v>21554.26</v>
-      </c>
-      <c r="W5" s="380"/>
-      <c r="X5" s="380"/>
+        <v>-21554.36</v>
+      </c>
+      <c r="R5" s="327">
+        <v>1146750</v>
+      </c>
+      <c r="S5" s="328" t="s">
+        <v>213</v>
+      </c>
+      <c r="W5" s="382"/>
+      <c r="X5" s="382"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15075,17 +15201,25 @@
       <c r="B6" s="24">
         <v>44537</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="25">
+        <v>12491</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>215</v>
+      </c>
       <c r="E6" s="27">
         <v>44537</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="28">
+        <v>71172</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="36">
         <v>44537</v>
       </c>
-      <c r="I6" s="30"/>
+      <c r="I6" s="30">
+        <v>700</v>
+      </c>
       <c r="J6" s="37"/>
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
@@ -15093,18 +15227,18 @@
         <v>0</v>
       </c>
       <c r="N6" s="33">
-        <v>0</v>
+        <v>35573</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="39">
         <f>N6+M6+L6+I6+C6</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="289">
+        <v>48764</v>
+      </c>
+      <c r="Q6" s="321">
         <f>P6-F6</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="229">
+        <v>-22408</v>
+      </c>
+      <c r="R6" s="323">
         <v>0</v>
       </c>
       <c r="S6" s="147"/>
@@ -15119,17 +15253,25 @@
       <c r="B7" s="24">
         <v>44538</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="40"/>
+      <c r="C7" s="25">
+        <v>36189.300000000003</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>218</v>
+      </c>
       <c r="E7" s="27">
         <v>44538</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="28">
+        <v>54679</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="36">
         <v>44538</v>
       </c>
-      <c r="I7" s="30"/>
+      <c r="I7" s="30">
+        <v>108</v>
+      </c>
       <c r="J7" s="37"/>
       <c r="K7" s="38"/>
       <c r="L7" s="39"/>
@@ -15137,21 +15279,24 @@
         <v>0</v>
       </c>
       <c r="N7" s="33">
-        <v>0</v>
+        <v>18382</v>
       </c>
       <c r="O7" s="224"/>
       <c r="P7" s="39">
         <f t="shared" ref="P7:P32" si="0">N7+M7+L7+I7+C7</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="289">
+        <v>54679.3</v>
+      </c>
+      <c r="Q7" s="321">
         <f t="shared" ref="Q7:Q35" si="1">P7-F7</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="229">
+        <v>0.30000000000291038</v>
+      </c>
+      <c r="R7" s="323">
         <v>0</v>
       </c>
       <c r="S7" s="147"/>
+      <c r="U7" s="1">
+        <v>12941.5</v>
+      </c>
       <c r="W7" s="234">
         <v>0</v>
       </c>
@@ -15163,17 +15308,25 @@
       <c r="B8" s="24">
         <v>44539</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="42"/>
+      <c r="C8" s="25">
+        <v>34279.21</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>219</v>
+      </c>
       <c r="E8" s="27">
         <v>44539</v>
       </c>
-      <c r="F8" s="28"/>
+      <c r="F8" s="28">
+        <v>73828</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="36">
         <v>44539</v>
       </c>
-      <c r="I8" s="30"/>
+      <c r="I8" s="30">
+        <v>120</v>
+      </c>
       <c r="J8" s="43"/>
       <c r="K8" s="38"/>
       <c r="L8" s="39"/>
@@ -15181,21 +15334,24 @@
         <v>0</v>
       </c>
       <c r="N8" s="33">
-        <v>0</v>
+        <v>39429</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="229">
+        <v>73828.209999999992</v>
+      </c>
+      <c r="Q8" s="321">
+        <f t="shared" si="1"/>
+        <v>0.20999999999185093</v>
+      </c>
+      <c r="R8" s="323">
         <v>0</v>
       </c>
       <c r="S8" s="147"/>
+      <c r="U8" s="1">
+        <v>19442</v>
+      </c>
       <c r="W8" s="234">
         <v>0</v>
       </c>
@@ -15207,36 +15363,44 @@
       <c r="B9" s="24">
         <v>44540</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="42"/>
+      <c r="C9" s="25">
+        <v>40355</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>220</v>
+      </c>
       <c r="E9" s="27">
         <v>44540</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="28">
+        <v>66009</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="36">
         <v>44540</v>
       </c>
-      <c r="I9" s="30"/>
+      <c r="I9" s="30">
+        <v>60</v>
+      </c>
       <c r="J9" s="37"/>
       <c r="K9" s="223"/>
       <c r="L9" s="39"/>
       <c r="M9" s="32">
-        <v>0</v>
+        <v>2970</v>
       </c>
       <c r="N9" s="33">
-        <v>0</v>
+        <v>22624</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="39">
         <f>N9+M9+L9+I9+C9</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="229">
+        <v>66009</v>
+      </c>
+      <c r="Q9" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R9" s="323">
         <v>0</v>
       </c>
       <c r="S9" s="147"/>
@@ -15251,36 +15415,45 @@
       <c r="B10" s="24">
         <v>44541</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="40"/>
+      <c r="C10" s="25">
+        <v>29815.61</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>221</v>
+      </c>
       <c r="E10" s="27">
         <v>44541</v>
       </c>
-      <c r="F10" s="28"/>
+      <c r="F10" s="28">
+        <v>71913</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="36">
         <v>44541</v>
       </c>
-      <c r="I10" s="30"/>
+      <c r="I10" s="30">
+        <v>3640</v>
+      </c>
       <c r="J10" s="37"/>
       <c r="K10" s="167"/>
       <c r="L10" s="45"/>
       <c r="M10" s="32">
-        <v>0</v>
+        <f>9785+2665</f>
+        <v>12450</v>
       </c>
       <c r="N10" s="33">
-        <v>0</v>
+        <v>26007</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="39">
         <f t="shared" ref="P10:P14" si="2">N10+M10+L10+I10+C10</f>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="229">
+        <v>71912.61</v>
+      </c>
+      <c r="Q10" s="321">
+        <f t="shared" si="1"/>
+        <v>-0.38999999999941792</v>
+      </c>
+      <c r="R10" s="323">
         <v>0</v>
       </c>
       <c r="S10" s="147"/>
@@ -15320,11 +15493,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="229">
+      <c r="Q11" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="323">
         <v>0</v>
       </c>
       <c r="S11" s="147"/>
@@ -15364,11 +15537,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="229">
+      <c r="Q12" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R12" s="323">
         <v>0</v>
       </c>
       <c r="S12" s="147"/>
@@ -15408,16 +15581,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="229">
-        <v>0</v>
-      </c>
-      <c r="S13" s="384"/>
+      <c r="Q13" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="323">
+        <v>0</v>
+      </c>
+      <c r="S13" s="320"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="U13" s="9"/>
       <c r="W13" s="234">
         <v>0</v>
       </c>
@@ -15454,11 +15627,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="229">
+      <c r="Q14" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R14" s="323">
         <v>0</v>
       </c>
       <c r="S14" s="147"/>
@@ -15497,11 +15670,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="229">
+      <c r="Q15" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="323">
         <v>0</v>
       </c>
       <c r="S15" s="147"/>
@@ -15540,11 +15713,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="229">
+      <c r="Q16" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="323">
         <v>0</v>
       </c>
       <c r="S16" s="147"/>
@@ -15583,11 +15756,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="229">
+      <c r="Q17" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="323">
         <v>0</v>
       </c>
       <c r="S17" s="147"/>
@@ -15626,11 +15799,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="229">
+      <c r="Q18" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="323">
         <v>0</v>
       </c>
       <c r="S18" s="147"/>
@@ -15669,15 +15842,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="229">
+      <c r="Q19" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="323">
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="375">
+      <c r="W19" s="386">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -15713,15 +15886,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="229">
+      <c r="Q20" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="323">
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="376"/>
+      <c r="W20" s="387"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -15754,16 +15927,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="229">
+      <c r="Q21" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="323">
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="377"/>
-      <c r="X21" s="377"/>
+      <c r="W21" s="388"/>
+      <c r="X21" s="388"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -15796,11 +15969,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="229">
+      <c r="Q22" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="323">
         <v>0</v>
       </c>
       <c r="S22" s="147"/>
@@ -15838,16 +16011,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="229">
+      <c r="Q23" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="323">
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="378"/>
-      <c r="X23" s="378"/>
+      <c r="W23" s="389"/>
+      <c r="X23" s="389"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -15880,16 +16053,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="229">
+      <c r="Q24" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R24" s="323">
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="378"/>
-      <c r="X24" s="378"/>
+      <c r="W24" s="389"/>
+      <c r="X24" s="389"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -15922,15 +16095,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="229">
-        <v>0</v>
-      </c>
-      <c r="W25" s="379"/>
-      <c r="X25" s="379"/>
+      <c r="Q25" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="323">
+        <v>0</v>
+      </c>
+      <c r="W25" s="390"/>
+      <c r="X25" s="390"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -15963,15 +16136,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="229">
-        <v>0</v>
-      </c>
-      <c r="W26" s="379"/>
-      <c r="X26" s="379"/>
+      <c r="Q26" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="323">
+        <v>0</v>
+      </c>
+      <c r="W26" s="390"/>
+      <c r="X26" s="390"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -16004,16 +16177,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="229">
-        <v>0</v>
-      </c>
-      <c r="W27" s="372"/>
-      <c r="X27" s="373"/>
-      <c r="Y27" s="374"/>
+      <c r="Q27" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="323">
+        <v>0</v>
+      </c>
+      <c r="W27" s="383"/>
+      <c r="X27" s="384"/>
+      <c r="Y27" s="385"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16045,16 +16218,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="229">
-        <v>0</v>
-      </c>
-      <c r="W28" s="373"/>
-      <c r="X28" s="373"/>
-      <c r="Y28" s="374"/>
+      <c r="Q28" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="323">
+        <v>0</v>
+      </c>
+      <c r="W28" s="384"/>
+      <c r="X28" s="384"/>
+      <c r="Y28" s="385"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16086,11 +16259,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="229">
+      <c r="Q29" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="323">
         <v>0</v>
       </c>
       <c r="W29" s="128"/>
@@ -16127,11 +16300,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="289">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="287"/>
+      <c r="Q30" s="321">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R30" s="324"/>
       <c r="X30" s="225"/>
       <c r="Y30" s="227"/>
     </row>
@@ -16168,7 +16341,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R31" s="287"/>
+      <c r="R31" s="325"/>
     </row>
     <row r="32" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23"/>
@@ -16308,21 +16481,21 @@
       <c r="J36" s="267"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="364">
+      <c r="M36" s="374">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
-        <v>1146750</v>
-      </c>
-      <c r="N36" s="366">
+        <v>15420</v>
+      </c>
+      <c r="N36" s="376">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
-        <v>36272</v>
+        <v>178287</v>
       </c>
       <c r="O36" s="277"/>
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="368">
+      <c r="Q36" s="378">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
-        <v>1125195.6399999999</v>
+        <v>-43962.240000000005</v>
       </c>
       <c r="R36" s="228"/>
     </row>
@@ -16339,13 +16512,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="365"/>
-      <c r="N37" s="367"/>
+      <c r="M37" s="375"/>
+      <c r="N37" s="377"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="369"/>
+      <c r="Q37" s="379"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -16386,7 +16559,7 @@
       <c r="N39" s="279"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>1193196.6399999999</v>
+        <v>361639.76</v>
       </c>
       <c r="Q39" s="276"/>
     </row>
@@ -16577,7 +16750,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>6888</v>
+        <v>160018.12</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -16585,7 +16758,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>68001</v>
+        <v>405602</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -16593,7 +16766,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>629.5</v>
+        <v>5257.5</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -16619,57 +16792,57 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="341" t="s">
+      <c r="H52" s="351" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="342"/>
+      <c r="I52" s="352"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="343">
+      <c r="K52" s="353">
         <f>I50+L50</f>
-        <v>3286.64</v>
-      </c>
-      <c r="L52" s="370"/>
+        <v>7914.6399999999994</v>
+      </c>
+      <c r="L52" s="380"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="347" t="s">
+      <c r="D53" s="357" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="347"/>
+      <c r="E53" s="357"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
-        <v>57826.36</v>
+        <v>237669.24</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="371" t="s">
+      <c r="D54" s="381" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="371"/>
+      <c r="E54" s="381"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="348" t="s">
+      <c r="I54" s="358" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="349"/>
-      <c r="K54" s="350">
+      <c r="J54" s="359"/>
+      <c r="K54" s="360">
         <f>F56+F57+F58</f>
-        <v>1392549.2600000002</v>
-      </c>
-      <c r="L54" s="350"/>
-      <c r="M54" s="356" t="s">
+        <v>1572392.1400000001</v>
+      </c>
+      <c r="L54" s="360"/>
+      <c r="M54" s="366" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="357"/>
-      <c r="O54" s="357"/>
-      <c r="P54" s="357"/>
-      <c r="Q54" s="358"/>
+      <c r="N54" s="367"/>
+      <c r="O54" s="367"/>
+      <c r="P54" s="367"/>
+      <c r="Q54" s="368"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -16683,11 +16856,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="359"/>
-      <c r="N55" s="360"/>
-      <c r="O55" s="360"/>
-      <c r="P55" s="360"/>
-      <c r="Q55" s="361"/>
+      <c r="M55" s="369"/>
+      <c r="N55" s="370"/>
+      <c r="O55" s="370"/>
+      <c r="P55" s="370"/>
+      <c r="Q55" s="371"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -16698,18 +16871,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-813787.36</v>
+        <v>-633944.48</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="352">
+      <c r="K56" s="362">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="353"/>
+      <c r="L56" s="363"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16726,22 +16899,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="330" t="s">
+      <c r="D58" s="340" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="331"/>
+      <c r="E58" s="341"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="332" t="s">
+      <c r="I58" s="342" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="333"/>
-      <c r="K58" s="334">
+      <c r="J58" s="343"/>
+      <c r="K58" s="344">
         <f>K54+K56</f>
-        <v>825159.91000000027</v>
-      </c>
-      <c r="L58" s="334"/>
+        <v>1005002.7900000002</v>
+      </c>
+      <c r="L58" s="344"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -16884,7 +17057,7 @@
       <c r="F80" s="129"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="30">
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -16907,6 +17080,7 @@
     <mergeCell ref="W23:X24"/>
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
+    <mergeCell ref="R3:R4"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:M1"/>
     <mergeCell ref="B3:C3"/>
@@ -16916,13 +17090,14 @@
     <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4021CBA2-E69D-45EC-899C-0BEE0EBDFE6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF6600FF"/>
   </sheetPr>
@@ -17011,7 +17186,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="295"/>
-      <c r="B3" s="383"/>
+      <c r="B3" s="319"/>
       <c r="C3" s="233"/>
       <c r="D3" s="298"/>
       <c r="E3" s="215"/>
@@ -18465,7 +18640,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="97"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="381" t="s">
+      <c r="F75" s="391" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -18478,7 +18653,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="97"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="382"/>
+      <c r="F76" s="392"/>
       <c r="K76" s="1"/>
       <c r="L76" s="97"/>
       <c r="M76" s="3"/>
@@ -18782,7 +18957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC9FF79-70F3-4EE5-BAC5-B7F8B481BD24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
cierre 28 dic 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="229">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -877,6 +877,27 @@
   </si>
   <si>
     <t>POLLO-QUESOS-LOMO-CHORIZO-PAVO</t>
+  </si>
+  <si>
+    <t>PAVOS--LONGANIZA</t>
+  </si>
+  <si>
+    <t>PAVOS</t>
+  </si>
+  <si>
+    <t>SALCHICHONERIA-ENCHILADA-ROAST BEFF-QUESOS</t>
+  </si>
+  <si>
+    <t>Transferencia  ODELPA</t>
+  </si>
+  <si>
+    <t>CHICHARRON-PULPA-SIRLON-POLLO-CHORIZO</t>
+  </si>
+  <si>
+    <t>POLLO-QUESO--LONGANIZA-ENCHILADA</t>
+  </si>
+  <si>
+    <t>CREMA-JAMON-POLLO-QUESOS-PIERNA-LONGANIZA-SALCHICHONERIA</t>
   </si>
 </sst>
 </file>
@@ -2478,7 +2499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="395">
+  <cellXfs count="399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3156,6 +3177,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3189,84 +3282,45 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3309,39 +3363,6 @@
     <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3354,6 +3375,12 @@
     <xf numFmtId="44" fontId="2" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -4956,23 +4983,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="329"/>
-      <c r="C1" s="331" t="s">
+      <c r="B1" s="353"/>
+      <c r="C1" s="355" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="332"/>
-      <c r="E1" s="332"/>
-      <c r="F1" s="332"/>
-      <c r="G1" s="332"/>
-      <c r="H1" s="332"/>
-      <c r="I1" s="332"/>
-      <c r="J1" s="332"/>
-      <c r="K1" s="332"/>
-      <c r="L1" s="332"/>
-      <c r="M1" s="332"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
+      <c r="I1" s="356"/>
+      <c r="J1" s="356"/>
+      <c r="K1" s="356"/>
+      <c r="L1" s="356"/>
+      <c r="M1" s="356"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="330"/>
+      <c r="B2" s="354"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -4982,17 +5009,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="333" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="334"/>
+      <c r="B3" s="357" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="358"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="335" t="s">
+      <c r="H3" s="359" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="335"/>
+      <c r="I3" s="359"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -5006,14 +5033,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="336" t="s">
+      <c r="E4" s="360" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="337"/>
-      <c r="H4" s="338" t="s">
+      <c r="F4" s="361"/>
+      <c r="H4" s="362" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="339"/>
+      <c r="I4" s="363"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -5023,10 +5050,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="345" t="s">
+      <c r="P4" s="334" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="346"/>
+      <c r="Q4" s="335"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -6467,11 +6494,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="347">
+      <c r="M39" s="336">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="349">
+      <c r="N39" s="338">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -6497,8 +6524,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="348"/>
-      <c r="N40" s="350"/>
+      <c r="M40" s="337"/>
+      <c r="N40" s="339"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -6713,29 +6740,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="351" t="s">
+      <c r="H52" s="340" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="352"/>
+      <c r="I52" s="341"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="353">
+      <c r="K52" s="342">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="354"/>
-      <c r="M52" s="355">
+      <c r="L52" s="343"/>
+      <c r="M52" s="344">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="356"/>
+      <c r="N52" s="345"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="346" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="346"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -6746,22 +6773,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="357" t="s">
+      <c r="D54" s="346" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="357"/>
+      <c r="E54" s="346"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="358" t="s">
+      <c r="I54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="359"/>
-      <c r="K54" s="360">
+      <c r="J54" s="348"/>
+      <c r="K54" s="349">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="361"/>
+      <c r="L54" s="350"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -6794,11 +6821,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="362">
+      <c r="K56" s="351">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="363"/>
+      <c r="L56" s="352"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -6815,22 +6842,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="340" t="s">
+      <c r="D58" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="341"/>
+      <c r="E58" s="330"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="342" t="s">
+      <c r="I58" s="331" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="343"/>
-      <c r="K58" s="344">
+      <c r="J58" s="332"/>
+      <c r="K58" s="333">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="344"/>
+      <c r="L58" s="333"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -6974,6 +7001,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -6988,12 +7021,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9962,23 +9989,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="329"/>
-      <c r="C1" s="331" t="s">
+      <c r="B1" s="353"/>
+      <c r="C1" s="355" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="332"/>
-      <c r="E1" s="332"/>
-      <c r="F1" s="332"/>
-      <c r="G1" s="332"/>
-      <c r="H1" s="332"/>
-      <c r="I1" s="332"/>
-      <c r="J1" s="332"/>
-      <c r="K1" s="332"/>
-      <c r="L1" s="332"/>
-      <c r="M1" s="332"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
+      <c r="I1" s="356"/>
+      <c r="J1" s="356"/>
+      <c r="K1" s="356"/>
+      <c r="L1" s="356"/>
+      <c r="M1" s="356"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="330"/>
+      <c r="B2" s="354"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -9988,21 +10015,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="333" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="334"/>
+      <c r="B3" s="357" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="358"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="335" t="s">
+      <c r="H3" s="359" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="335"/>
+      <c r="I3" s="359"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="372" t="s">
+      <c r="P3" s="383" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10017,14 +10044,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="336" t="s">
+      <c r="E4" s="360" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="337"/>
-      <c r="H4" s="338" t="s">
+      <c r="F4" s="361"/>
+      <c r="H4" s="362" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="339"/>
+      <c r="I4" s="363"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -10034,14 +10061,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="373"/>
+      <c r="P4" s="384"/>
       <c r="Q4" s="288" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="382" t="s">
+      <c r="W4" s="366" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="382"/>
+      <c r="X4" s="366"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10092,8 +10119,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="382"/>
-      <c r="X5" s="382"/>
+      <c r="W5" s="366"/>
+      <c r="X5" s="366"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10864,7 +10891,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="386">
+      <c r="W19" s="370">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -10916,7 +10943,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="387"/>
+      <c r="W20" s="371"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -10965,8 +10992,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="388"/>
-      <c r="X21" s="388"/>
+      <c r="W21" s="372"/>
+      <c r="X21" s="372"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -11067,8 +11094,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="389"/>
-      <c r="X23" s="389"/>
+      <c r="W23" s="373"/>
+      <c r="X23" s="373"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -11122,8 +11149,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="389"/>
-      <c r="X24" s="389"/>
+      <c r="W24" s="373"/>
+      <c r="X24" s="373"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -11169,8 +11196,8 @@
       <c r="R25" s="287">
         <v>28952</v>
       </c>
-      <c r="W25" s="390"/>
-      <c r="X25" s="390"/>
+      <c r="W25" s="374"/>
+      <c r="X25" s="374"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -11221,8 +11248,8 @@
       <c r="R26" s="287">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="390"/>
-      <c r="X26" s="390"/>
+      <c r="W26" s="374"/>
+      <c r="X26" s="374"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -11270,9 +11297,9 @@
       <c r="R27" s="287">
         <v>14637</v>
       </c>
-      <c r="W27" s="383"/>
-      <c r="X27" s="384"/>
-      <c r="Y27" s="385"/>
+      <c r="W27" s="367"/>
+      <c r="X27" s="368"/>
+      <c r="Y27" s="369"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11322,9 +11349,9 @@
       <c r="R28" s="287">
         <v>0</v>
       </c>
-      <c r="W28" s="384"/>
-      <c r="X28" s="384"/>
-      <c r="Y28" s="385"/>
+      <c r="W28" s="368"/>
+      <c r="X28" s="368"/>
+      <c r="Y28" s="369"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11659,11 +11686,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="374">
+      <c r="M36" s="385">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="376">
+      <c r="N36" s="387">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -11671,7 +11698,7 @@
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="378">
+      <c r="Q36" s="389">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -11706,13 +11733,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="375"/>
-      <c r="N37" s="377"/>
+      <c r="M37" s="386"/>
+      <c r="N37" s="388"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="379"/>
+      <c r="Q37" s="390"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -12002,26 +12029,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="351" t="s">
+      <c r="H52" s="340" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="352"/>
+      <c r="I52" s="341"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="353">
+      <c r="K52" s="342">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="380"/>
+      <c r="L52" s="375"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="346" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="346"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -12030,29 +12057,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="381" t="s">
+      <c r="D54" s="376" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="381"/>
+      <c r="E54" s="376"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="358" t="s">
+      <c r="I54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="359"/>
-      <c r="K54" s="360">
+      <c r="J54" s="348"/>
+      <c r="K54" s="349">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="360"/>
-      <c r="M54" s="366" t="s">
+      <c r="L54" s="349"/>
+      <c r="M54" s="377" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="367"/>
-      <c r="O54" s="367"/>
-      <c r="P54" s="367"/>
-      <c r="Q54" s="368"/>
+      <c r="N54" s="378"/>
+      <c r="O54" s="378"/>
+      <c r="P54" s="378"/>
+      <c r="Q54" s="379"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -12066,11 +12093,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="369"/>
-      <c r="N55" s="370"/>
-      <c r="O55" s="370"/>
-      <c r="P55" s="370"/>
-      <c r="Q55" s="371"/>
+      <c r="M55" s="380"/>
+      <c r="N55" s="381"/>
+      <c r="O55" s="381"/>
+      <c r="P55" s="381"/>
+      <c r="Q55" s="382"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -12088,11 +12115,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="362">
+      <c r="K56" s="351">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="363"/>
+      <c r="L56" s="352"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -12109,22 +12136,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="340" t="s">
+      <c r="D58" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="341"/>
+      <c r="E58" s="330"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="342" t="s">
+      <c r="I58" s="331" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="343"/>
-      <c r="K58" s="344">
+      <c r="J58" s="332"/>
+      <c r="K58" s="333">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="344"/>
+      <c r="L58" s="333"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -12268,14 +12295,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -12286,17 +12316,14 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15018,8 +15045,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15042,29 +15069,29 @@
     <col min="17" max="17" width="18.140625" style="225" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="227" customWidth="1"/>
     <col min="19" max="20" width="11.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="329"/>
-      <c r="C1" s="331" t="s">
+      <c r="B1" s="353"/>
+      <c r="C1" s="355" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="332"/>
-      <c r="E1" s="332"/>
-      <c r="F1" s="332"/>
-      <c r="G1" s="332"/>
-      <c r="H1" s="332"/>
-      <c r="I1" s="332"/>
-      <c r="J1" s="332"/>
-      <c r="K1" s="332"/>
-      <c r="L1" s="332"/>
-      <c r="M1" s="332"/>
+      <c r="D1" s="356"/>
+      <c r="E1" s="356"/>
+      <c r="F1" s="356"/>
+      <c r="G1" s="356"/>
+      <c r="H1" s="356"/>
+      <c r="I1" s="356"/>
+      <c r="J1" s="356"/>
+      <c r="K1" s="356"/>
+      <c r="L1" s="356"/>
+      <c r="M1" s="356"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="330"/>
+      <c r="B2" s="354"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -15074,21 +15101,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="333" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="334"/>
+      <c r="B3" s="357" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="358"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="335" t="s">
+      <c r="H3" s="359" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="335"/>
+      <c r="I3" s="359"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="372" t="s">
+      <c r="P3" s="383" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="393" t="s">
@@ -15106,14 +15133,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="336" t="s">
+      <c r="E4" s="360" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="337"/>
-      <c r="H4" s="338" t="s">
+      <c r="F4" s="361"/>
+      <c r="H4" s="362" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="339"/>
+      <c r="I4" s="363"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -15123,15 +15150,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="373"/>
+      <c r="P4" s="384"/>
       <c r="Q4" s="326" t="s">
         <v>217</v>
       </c>
       <c r="R4" s="394"/>
-      <c r="W4" s="382" t="s">
+      <c r="W4" s="366" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="382"/>
+      <c r="X4" s="366"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15172,7 +15199,7 @@
         <v>2657.14</v>
       </c>
       <c r="M5" s="32">
-        <v>0</v>
+        <v>21554.5</v>
       </c>
       <c r="N5" s="33">
         <v>36272</v>
@@ -15180,11 +15207,11 @@
       <c r="O5" s="322"/>
       <c r="P5" s="34">
         <f>N5+M5+L5+I5+C5</f>
-        <v>46446.64</v>
-      </c>
-      <c r="Q5" s="321">
+        <v>68001.14</v>
+      </c>
+      <c r="Q5" s="395">
         <f>P5-F5</f>
-        <v>-21554.36</v>
+        <v>0.13999999999941792</v>
       </c>
       <c r="R5" s="327">
         <v>1146750</v>
@@ -15192,8 +15219,8 @@
       <c r="S5" s="328" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="382"/>
-      <c r="X5" s="382"/>
+      <c r="W5" s="366"/>
+      <c r="X5" s="366"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15224,7 +15251,7 @@
       <c r="K6" s="38"/>
       <c r="L6" s="39"/>
       <c r="M6" s="32">
-        <v>0</v>
+        <v>22408</v>
       </c>
       <c r="N6" s="33">
         <v>35573</v>
@@ -15232,16 +15259,19 @@
       <c r="O6" s="2"/>
       <c r="P6" s="39">
         <f>N6+M6+L6+I6+C6</f>
-        <v>48764</v>
-      </c>
-      <c r="Q6" s="321">
+        <v>71172</v>
+      </c>
+      <c r="Q6" s="395">
         <f>P6-F6</f>
-        <v>-22408</v>
+        <v>0</v>
       </c>
       <c r="R6" s="323">
         <v>0</v>
       </c>
       <c r="S6" s="147"/>
+      <c r="U6" s="396" t="s">
+        <v>223</v>
+      </c>
       <c r="W6" s="234">
         <v>0</v>
       </c>
@@ -15294,7 +15324,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="147"/>
-      <c r="U7" s="1">
+      <c r="U7" s="397">
         <v>12941.5</v>
       </c>
       <c r="W7" s="234">
@@ -15349,7 +15379,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="147"/>
-      <c r="U8" s="1">
+      <c r="U8" s="397">
         <v>19442</v>
       </c>
       <c r="W8" s="234">
@@ -15404,6 +15434,9 @@
         <v>0</v>
       </c>
       <c r="S9" s="147"/>
+      <c r="U9" s="397">
+        <v>36844</v>
+      </c>
       <c r="W9" s="234">
         <v>0</v>
       </c>
@@ -15457,6 +15490,9 @@
         <v>0</v>
       </c>
       <c r="S10" s="147"/>
+      <c r="U10" s="397">
+        <v>22942</v>
+      </c>
       <c r="W10" s="234">
         <v>0</v>
       </c>
@@ -15468,30 +15504,38 @@
       <c r="B11" s="24">
         <v>44542</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="35"/>
+      <c r="C11" s="25">
+        <v>20722</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>222</v>
+      </c>
       <c r="E11" s="27">
         <v>44542</v>
       </c>
-      <c r="F11" s="28"/>
+      <c r="F11" s="28">
+        <v>52385</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="36">
         <v>44542</v>
       </c>
-      <c r="I11" s="30"/>
+      <c r="I11" s="30">
+        <v>3991</v>
+      </c>
       <c r="J11" s="43"/>
       <c r="K11" s="168"/>
       <c r="L11" s="39"/>
       <c r="M11" s="32">
-        <v>0</v>
+        <v>9148</v>
       </c>
       <c r="N11" s="33">
-        <v>0</v>
+        <v>18524</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>52385</v>
       </c>
       <c r="Q11" s="321">
         <f t="shared" si="1"/>
@@ -15501,6 +15545,9 @@
         <v>0</v>
       </c>
       <c r="S11" s="147"/>
+      <c r="U11" s="397">
+        <v>15322.5</v>
+      </c>
       <c r="W11" s="234">
         <v>0</v>
       </c>
@@ -15512,30 +15559,41 @@
       <c r="B12" s="24">
         <v>44543</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="35"/>
+      <c r="C12" s="25">
+        <v>7052</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>224</v>
+      </c>
       <c r="E12" s="27">
         <v>44543</v>
       </c>
-      <c r="F12" s="28"/>
+      <c r="F12" s="28">
+        <v>69062</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="36">
         <v>44543</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="30">
+        <v>0</v>
+      </c>
       <c r="J12" s="37"/>
       <c r="K12" s="169"/>
       <c r="L12" s="39"/>
       <c r="M12" s="32">
-        <v>0</v>
+        <f>31028+1388</f>
+        <v>32416</v>
       </c>
       <c r="N12" s="33">
-        <v>0</v>
-      </c>
-      <c r="O12" s="2"/>
+        <v>29594</v>
+      </c>
+      <c r="O12" s="398" t="s">
+        <v>225</v>
+      </c>
       <c r="P12" s="39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>69062</v>
       </c>
       <c r="Q12" s="321">
         <f t="shared" si="1"/>
@@ -15545,6 +15603,10 @@
         <v>0</v>
       </c>
       <c r="S12" s="147"/>
+      <c r="U12" s="1">
+        <f>SUM(U7:U11)</f>
+        <v>107492</v>
+      </c>
       <c r="W12" s="234">
         <v>0</v>
       </c>
@@ -15556,30 +15618,39 @@
       <c r="B13" s="24">
         <v>44544</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="25">
+        <v>27597.5</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>226</v>
+      </c>
       <c r="E13" s="27">
         <v>44544</v>
       </c>
-      <c r="F13" s="28"/>
+      <c r="F13" s="28">
+        <v>77884</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="36">
         <v>44544</v>
       </c>
-      <c r="I13" s="30"/>
+      <c r="I13" s="30">
+        <v>1334</v>
+      </c>
       <c r="J13" s="37"/>
       <c r="K13" s="38"/>
       <c r="L13" s="39"/>
       <c r="M13" s="32">
-        <v>0</v>
+        <f>933+12801.5</f>
+        <v>13734.5</v>
       </c>
       <c r="N13" s="33">
-        <v>0</v>
+        <v>35218</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>77884</v>
       </c>
       <c r="Q13" s="321">
         <f t="shared" si="1"/>
@@ -15602,34 +15673,43 @@
       <c r="B14" s="24">
         <v>44545</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="40"/>
+      <c r="C14" s="25">
+        <v>13752</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>227</v>
+      </c>
       <c r="E14" s="27">
         <v>44545</v>
       </c>
-      <c r="F14" s="28"/>
+      <c r="F14" s="28">
+        <v>91827</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="36">
         <v>44545</v>
       </c>
-      <c r="I14" s="30"/>
+      <c r="I14" s="30">
+        <v>1641</v>
+      </c>
       <c r="J14" s="37"/>
       <c r="K14" s="38"/>
       <c r="L14" s="39"/>
       <c r="M14" s="32">
-        <v>0</v>
+        <f>55316+466.8+1331</f>
+        <v>57113.8</v>
       </c>
       <c r="N14" s="33">
-        <v>0</v>
+        <v>19320</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="39">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>91826.8</v>
       </c>
       <c r="Q14" s="321">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.19999999999708962</v>
       </c>
       <c r="R14" s="323">
         <v>0</v>
@@ -15646,29 +15726,38 @@
       <c r="B15" s="24">
         <v>44546</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="40"/>
+      <c r="C15" s="25">
+        <v>15710</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>228</v>
+      </c>
       <c r="E15" s="27">
         <v>44546</v>
       </c>
-      <c r="F15" s="28"/>
+      <c r="F15" s="28">
+        <v>93120</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="36">
         <v>44546</v>
       </c>
-      <c r="I15" s="30"/>
+      <c r="I15" s="30">
+        <v>75</v>
+      </c>
       <c r="J15" s="37"/>
       <c r="K15" s="38"/>
       <c r="L15" s="39"/>
       <c r="M15" s="32">
-        <v>0</v>
+        <f>33682+1408</f>
+        <v>35090</v>
       </c>
       <c r="N15" s="33">
-        <v>0</v>
+        <v>42245</v>
       </c>
       <c r="P15" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>93120</v>
       </c>
       <c r="Q15" s="321">
         <f t="shared" si="1"/>
@@ -15689,33 +15778,42 @@
       <c r="B16" s="24">
         <v>44547</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="35"/>
+      <c r="C16" s="25">
+        <v>2467</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>112</v>
+      </c>
       <c r="E16" s="27">
         <v>44547</v>
       </c>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28">
+        <v>93493</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="36">
         <v>44547</v>
       </c>
-      <c r="I16" s="30"/>
+      <c r="I16" s="30">
+        <v>240</v>
+      </c>
       <c r="J16" s="37"/>
       <c r="K16" s="169"/>
       <c r="L16" s="9"/>
       <c r="M16" s="32">
-        <v>0</v>
+        <f>58263+49100</f>
+        <v>107363</v>
       </c>
       <c r="N16" s="33">
-        <v>0</v>
+        <v>32523</v>
       </c>
       <c r="P16" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>142593</v>
       </c>
       <c r="Q16" s="321">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>49100</v>
       </c>
       <c r="R16" s="323">
         <v>0</v>
@@ -15850,7 +15948,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="386">
+      <c r="W19" s="370">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -15894,7 +15992,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="387"/>
+      <c r="W20" s="371"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -15935,8 +16033,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="388"/>
-      <c r="X21" s="388"/>
+      <c r="W21" s="372"/>
+      <c r="X21" s="372"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -16019,8 +16117,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="389"/>
-      <c r="X23" s="389"/>
+      <c r="W23" s="373"/>
+      <c r="X23" s="373"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -16061,8 +16159,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="389"/>
-      <c r="X24" s="389"/>
+      <c r="W24" s="373"/>
+      <c r="X24" s="373"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -16102,8 +16200,8 @@
       <c r="R25" s="323">
         <v>0</v>
       </c>
-      <c r="W25" s="390"/>
-      <c r="X25" s="390"/>
+      <c r="W25" s="374"/>
+      <c r="X25" s="374"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -16143,8 +16241,8 @@
       <c r="R26" s="323">
         <v>0</v>
       </c>
-      <c r="W26" s="390"/>
-      <c r="X26" s="390"/>
+      <c r="W26" s="374"/>
+      <c r="X26" s="374"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -16184,9 +16282,9 @@
       <c r="R27" s="323">
         <v>0</v>
       </c>
-      <c r="W27" s="383"/>
-      <c r="X27" s="384"/>
-      <c r="Y27" s="385"/>
+      <c r="W27" s="367"/>
+      <c r="X27" s="368"/>
+      <c r="Y27" s="369"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16225,9 +16323,9 @@
       <c r="R28" s="323">
         <v>0</v>
       </c>
-      <c r="W28" s="384"/>
-      <c r="X28" s="384"/>
-      <c r="Y28" s="385"/>
+      <c r="W28" s="368"/>
+      <c r="X28" s="368"/>
+      <c r="Y28" s="369"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16481,21 +16579,21 @@
       <c r="J36" s="267"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="374">
+      <c r="M36" s="385">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
-        <v>15420</v>
-      </c>
-      <c r="N36" s="376">
+        <v>314247.8</v>
+      </c>
+      <c r="N36" s="387">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
-        <v>178287</v>
+        <v>355711</v>
       </c>
       <c r="O36" s="277"/>
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="378">
+      <c r="Q36" s="389">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
-        <v>-43962.240000000005</v>
+        <v>49100.06</v>
       </c>
       <c r="R36" s="228"/>
     </row>
@@ -16512,13 +16610,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="375"/>
-      <c r="N37" s="377"/>
+      <c r="M37" s="386"/>
+      <c r="N37" s="388"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="379"/>
+      <c r="Q37" s="390"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -16559,7 +16657,7 @@
       <c r="N39" s="279"/>
       <c r="P39" s="34">
         <f>SUM(P5:P38)</f>
-        <v>361639.76</v>
+        <v>932473.06</v>
       </c>
       <c r="Q39" s="276"/>
     </row>
@@ -16750,7 +16848,7 @@
       </c>
       <c r="C50" s="87">
         <f>SUM(C5:C49)</f>
-        <v>160018.12</v>
+        <v>247318.62</v>
       </c>
       <c r="D50" s="88"/>
       <c r="E50" s="89" t="s">
@@ -16758,7 +16856,7 @@
       </c>
       <c r="F50" s="90">
         <f>SUM(F5:F49)</f>
-        <v>405602</v>
+        <v>883373</v>
       </c>
       <c r="G50" s="88"/>
       <c r="H50" s="91" t="s">
@@ -16766,7 +16864,7 @@
       </c>
       <c r="I50" s="92">
         <f>SUM(I5:I49)</f>
-        <v>5257.5</v>
+        <v>12538.5</v>
       </c>
       <c r="J50" s="93"/>
       <c r="K50" s="94" t="s">
@@ -16792,57 +16890,57 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="351" t="s">
+      <c r="H52" s="340" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="352"/>
+      <c r="I52" s="341"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="353">
+      <c r="K52" s="342">
         <f>I50+L50</f>
-        <v>7914.6399999999994</v>
-      </c>
-      <c r="L52" s="380"/>
+        <v>15195.64</v>
+      </c>
+      <c r="L52" s="375"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="357" t="s">
+      <c r="D53" s="346" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="357"/>
+      <c r="E53" s="346"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
-        <v>237669.24</v>
+        <v>620858.74</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="381" t="s">
+      <c r="D54" s="376" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="381"/>
+      <c r="E54" s="376"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="358" t="s">
+      <c r="I54" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="359"/>
-      <c r="K54" s="360">
+      <c r="J54" s="348"/>
+      <c r="K54" s="349">
         <f>F56+F57+F58</f>
-        <v>1572392.1400000001</v>
-      </c>
-      <c r="L54" s="360"/>
-      <c r="M54" s="366" t="s">
+        <v>1955581.6400000001</v>
+      </c>
+      <c r="L54" s="349"/>
+      <c r="M54" s="377" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="367"/>
-      <c r="O54" s="367"/>
-      <c r="P54" s="367"/>
-      <c r="Q54" s="368"/>
+      <c r="N54" s="378"/>
+      <c r="O54" s="378"/>
+      <c r="P54" s="378"/>
+      <c r="Q54" s="379"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -16856,11 +16954,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="369"/>
-      <c r="N55" s="370"/>
-      <c r="O55" s="370"/>
-      <c r="P55" s="370"/>
-      <c r="Q55" s="371"/>
+      <c r="M55" s="380"/>
+      <c r="N55" s="381"/>
+      <c r="O55" s="381"/>
+      <c r="P55" s="381"/>
+      <c r="Q55" s="382"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -16871,18 +16969,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-633944.48</v>
+        <v>-250754.98</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="362">
+      <c r="K56" s="351">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="363"/>
+      <c r="L56" s="352"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -16899,22 +16997,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="340" t="s">
+      <c r="D58" s="329" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="341"/>
+      <c r="E58" s="330"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="342" t="s">
+      <c r="I58" s="331" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="343"/>
-      <c r="K58" s="344">
+      <c r="J58" s="332"/>
+      <c r="K58" s="333">
         <f>K54+K56</f>
-        <v>1005002.7900000002</v>
-      </c>
-      <c r="L58" s="344"/>
+        <v>1388192.29</v>
+      </c>
+      <c r="L58" s="333"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -17058,20 +17156,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -17081,13 +17172,20 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 14 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE    ZAVALETA   DICIEMBRE     2021.xlsx
@@ -3527,204 +3527,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="47" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3767,6 +3569,204 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="38" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="14" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="33" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="77" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="3" borderId="71" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="70" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="3" borderId="72" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="41" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="74" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="17" borderId="82" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -5369,23 +5369,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="351"/>
-      <c r="C1" s="353" t="s">
+      <c r="B1" s="395"/>
+      <c r="C1" s="397" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="354"/>
-      <c r="E1" s="354"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
-      <c r="H1" s="354"/>
-      <c r="I1" s="354"/>
-      <c r="J1" s="354"/>
-      <c r="K1" s="354"/>
-      <c r="L1" s="354"/>
-      <c r="M1" s="354"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="398"/>
+      <c r="G1" s="398"/>
+      <c r="H1" s="398"/>
+      <c r="I1" s="398"/>
+      <c r="J1" s="398"/>
+      <c r="K1" s="398"/>
+      <c r="L1" s="398"/>
+      <c r="M1" s="398"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="352"/>
+      <c r="B2" s="396"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -5395,17 +5395,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="355" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="356"/>
+      <c r="B3" s="399" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="400"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="357" t="s">
+      <c r="H3" s="401" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="357"/>
+      <c r="I3" s="401"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -5419,14 +5419,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="358" t="s">
+      <c r="E4" s="402" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="359"/>
-      <c r="H4" s="360" t="s">
+      <c r="F4" s="403"/>
+      <c r="H4" s="404" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="361"/>
+      <c r="I4" s="405"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -5436,10 +5436,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="367" t="s">
+      <c r="P4" s="376" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="368"/>
+      <c r="Q4" s="377"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -6880,11 +6880,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="177"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="369">
+      <c r="M39" s="378">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="371">
+      <c r="N39" s="380">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -6910,8 +6910,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="370"/>
-      <c r="N40" s="372"/>
+      <c r="M40" s="379"/>
+      <c r="N40" s="381"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -7126,29 +7126,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="373" t="s">
+      <c r="H52" s="382" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="374"/>
+      <c r="I52" s="383"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="375">
+      <c r="K52" s="384">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="376"/>
-      <c r="M52" s="377">
+      <c r="L52" s="385"/>
+      <c r="M52" s="386">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="378"/>
+      <c r="N52" s="387"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="379" t="s">
+      <c r="D53" s="388" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="379"/>
+      <c r="E53" s="388"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -7159,22 +7159,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="379" t="s">
+      <c r="D54" s="388" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="379"/>
+      <c r="E54" s="388"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="380" t="s">
+      <c r="I54" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="381"/>
-      <c r="K54" s="382">
+      <c r="J54" s="390"/>
+      <c r="K54" s="391">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="383"/>
+      <c r="L54" s="392"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -7207,11 +7207,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="384">
+      <c r="K56" s="393">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="385"/>
+      <c r="L56" s="394"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -7228,22 +7228,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="362" t="s">
+      <c r="D58" s="371" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="363"/>
+      <c r="E58" s="372"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="364" t="s">
+      <c r="I58" s="373" t="s">
         <v>97</v>
       </c>
-      <c r="J58" s="365"/>
-      <c r="K58" s="366">
+      <c r="J58" s="374"/>
+      <c r="K58" s="375">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="366"/>
+      <c r="L58" s="375"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -7387,6 +7387,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -7401,12 +7407,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -8747,7 +8747,7 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="386" t="s">
+      <c r="B41" s="406" t="s">
         <v>92</v>
       </c>
       <c r="C41" s="190">
@@ -8779,7 +8779,7 @@
       <c r="A42" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="387"/>
+      <c r="B42" s="407"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -10375,23 +10375,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="351"/>
-      <c r="C1" s="353" t="s">
+      <c r="B1" s="395"/>
+      <c r="C1" s="397" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="354"/>
-      <c r="E1" s="354"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
-      <c r="H1" s="354"/>
-      <c r="I1" s="354"/>
-      <c r="J1" s="354"/>
-      <c r="K1" s="354"/>
-      <c r="L1" s="354"/>
-      <c r="M1" s="354"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="398"/>
+      <c r="G1" s="398"/>
+      <c r="H1" s="398"/>
+      <c r="I1" s="398"/>
+      <c r="J1" s="398"/>
+      <c r="K1" s="398"/>
+      <c r="L1" s="398"/>
+      <c r="M1" s="398"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="352"/>
+      <c r="B2" s="396"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -10401,21 +10401,21 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="355" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="356"/>
+      <c r="B3" s="399" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="400"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="357" t="s">
+      <c r="H3" s="401" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="357"/>
+      <c r="I3" s="401"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="394" t="s">
+      <c r="P3" s="425" t="s">
         <v>6</v>
       </c>
     </row>
@@ -10430,14 +10430,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="358" t="s">
+      <c r="E4" s="402" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="359"/>
-      <c r="H4" s="360" t="s">
+      <c r="F4" s="403"/>
+      <c r="H4" s="404" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="361"/>
+      <c r="I4" s="405"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -10447,14 +10447,14 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="395"/>
+      <c r="P4" s="426"/>
       <c r="Q4" s="288" t="s">
         <v>209</v>
       </c>
-      <c r="W4" s="404" t="s">
+      <c r="W4" s="408" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="404"/>
+      <c r="X4" s="408"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -10505,8 +10505,8 @@
         <f>20000+7936</f>
         <v>27936</v>
       </c>
-      <c r="W5" s="404"/>
-      <c r="X5" s="404"/>
+      <c r="W5" s="408"/>
+      <c r="X5" s="408"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11277,7 +11277,7 @@
         <v>26370</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="408">
+      <c r="W19" s="412">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>935136</v>
       </c>
@@ -11329,7 +11329,7 @@
         <v>16395.830000000002</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="409"/>
+      <c r="W20" s="413"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -11378,8 +11378,8 @@
         <v>19188.82</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="410"/>
-      <c r="X21" s="410"/>
+      <c r="W21" s="414"/>
+      <c r="X21" s="414"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -11480,8 +11480,8 @@
         <v>45217.29</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="411"/>
-      <c r="X23" s="411"/>
+      <c r="W23" s="415"/>
+      <c r="X23" s="415"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -11535,8 +11535,8 @@
         <v>23159.17</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="411"/>
-      <c r="X24" s="411"/>
+      <c r="W24" s="415"/>
+      <c r="X24" s="415"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -11582,8 +11582,8 @@
       <c r="R25" s="287">
         <v>28952</v>
       </c>
-      <c r="W25" s="412"/>
-      <c r="X25" s="412"/>
+      <c r="W25" s="416"/>
+      <c r="X25" s="416"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -11634,8 +11634,8 @@
       <c r="R26" s="287">
         <v>21771.5</v>
       </c>
-      <c r="W26" s="412"/>
-      <c r="X26" s="412"/>
+      <c r="W26" s="416"/>
+      <c r="X26" s="416"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -11683,9 +11683,9 @@
       <c r="R27" s="287">
         <v>14637</v>
       </c>
-      <c r="W27" s="405"/>
-      <c r="X27" s="406"/>
-      <c r="Y27" s="407"/>
+      <c r="W27" s="409"/>
+      <c r="X27" s="410"/>
+      <c r="Y27" s="411"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -11735,9 +11735,9 @@
       <c r="R28" s="287">
         <v>0</v>
       </c>
-      <c r="W28" s="406"/>
-      <c r="X28" s="406"/>
-      <c r="Y28" s="407"/>
+      <c r="W28" s="410"/>
+      <c r="X28" s="410"/>
+      <c r="Y28" s="411"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -12072,11 +12072,11 @@
       <c r="L36" s="44">
         <v>5940</v>
       </c>
-      <c r="M36" s="396">
+      <c r="M36" s="427">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>321168.83</v>
       </c>
-      <c r="N36" s="398">
+      <c r="N36" s="429">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>467016</v>
       </c>
@@ -12084,7 +12084,7 @@
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="400">
+      <c r="Q36" s="431">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-637069.14000000013</v>
       </c>
@@ -12119,13 +12119,13 @@
       <c r="L37" s="61">
         <v>7929.62</v>
       </c>
-      <c r="M37" s="397"/>
-      <c r="N37" s="399"/>
+      <c r="M37" s="428"/>
+      <c r="N37" s="430"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="401"/>
+      <c r="Q37" s="432"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -12415,26 +12415,26 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="373" t="s">
+      <c r="H52" s="382" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="374"/>
+      <c r="I52" s="383"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="375">
+      <c r="K52" s="384">
         <f>I50+L50</f>
         <v>71911.59</v>
       </c>
-      <c r="L52" s="402"/>
+      <c r="L52" s="417"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="379" t="s">
+      <c r="D53" s="388" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="379"/>
+      <c r="E53" s="388"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
         <v>-25952.549999999814</v>
@@ -12443,29 +12443,29 @@
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="403" t="s">
+      <c r="D54" s="418" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="403"/>
+      <c r="E54" s="418"/>
       <c r="F54" s="111">
         <v>-706888.38</v>
       </c>
-      <c r="I54" s="380" t="s">
+      <c r="I54" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="381"/>
-      <c r="K54" s="382">
+      <c r="J54" s="390"/>
+      <c r="K54" s="391">
         <f>F56+F57+F58</f>
         <v>1308778.3500000003</v>
       </c>
-      <c r="L54" s="382"/>
-      <c r="M54" s="388" t="s">
+      <c r="L54" s="391"/>
+      <c r="M54" s="419" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="389"/>
-      <c r="O54" s="389"/>
-      <c r="P54" s="389"/>
-      <c r="Q54" s="390"/>
+      <c r="N54" s="420"/>
+      <c r="O54" s="420"/>
+      <c r="P54" s="420"/>
+      <c r="Q54" s="421"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -12479,11 +12479,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="391"/>
-      <c r="N55" s="392"/>
-      <c r="O55" s="392"/>
-      <c r="P55" s="392"/>
-      <c r="Q55" s="393"/>
+      <c r="M55" s="422"/>
+      <c r="N55" s="423"/>
+      <c r="O55" s="423"/>
+      <c r="P55" s="423"/>
+      <c r="Q55" s="424"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -12501,11 +12501,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="384">
+      <c r="K56" s="393">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="385"/>
+      <c r="L56" s="394"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -12522,22 +12522,22 @@
       <c r="C58" s="112">
         <v>44535</v>
       </c>
-      <c r="D58" s="362" t="s">
+      <c r="D58" s="371" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="363"/>
+      <c r="E58" s="372"/>
       <c r="F58" s="113">
         <v>2142307.62</v>
       </c>
-      <c r="I58" s="364" t="s">
+      <c r="I58" s="373" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="365"/>
-      <c r="K58" s="366">
+      <c r="J58" s="374"/>
+      <c r="K58" s="375">
         <f>K54+K56</f>
         <v>741389.00000000035</v>
       </c>
-      <c r="L58" s="366"/>
+      <c r="L58" s="375"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -12681,14 +12681,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="W4:X5"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W23:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -12699,17 +12702,14 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="W4:X5"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W23:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="0.15748031496062992" right="0.15748031496062992" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="68" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -15108,7 +15108,7 @@
       <c r="C87" s="214"/>
       <c r="D87" s="97"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="413" t="s">
+      <c r="F87" s="433" t="s">
         <v>207</v>
       </c>
       <c r="K87" s="1"/>
@@ -15121,7 +15121,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="97"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="414"/>
+      <c r="F88" s="434"/>
       <c r="K88" s="1"/>
       <c r="L88" s="97"/>
       <c r="M88" s="3"/>
@@ -15431,8 +15431,8 @@
   </sheetPr>
   <dimension ref="A1:Z80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15461,23 +15461,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="351"/>
-      <c r="C1" s="353" t="s">
+      <c r="B1" s="395"/>
+      <c r="C1" s="397" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="354"/>
-      <c r="E1" s="354"/>
-      <c r="F1" s="354"/>
-      <c r="G1" s="354"/>
-      <c r="H1" s="354"/>
-      <c r="I1" s="354"/>
-      <c r="J1" s="354"/>
-      <c r="K1" s="354"/>
-      <c r="L1" s="354"/>
-      <c r="M1" s="354"/>
+      <c r="D1" s="398"/>
+      <c r="E1" s="398"/>
+      <c r="F1" s="398"/>
+      <c r="G1" s="398"/>
+      <c r="H1" s="398"/>
+      <c r="I1" s="398"/>
+      <c r="J1" s="398"/>
+      <c r="K1" s="398"/>
+      <c r="L1" s="398"/>
+      <c r="M1" s="398"/>
     </row>
     <row r="2" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="352"/>
+      <c r="B2" s="396"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -15487,24 +15487,24 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="355" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="356"/>
+      <c r="B3" s="399" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="400"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="357" t="s">
+      <c r="H3" s="401" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="357"/>
+      <c r="I3" s="401"/>
       <c r="K3" s="165"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
-      <c r="P3" s="394" t="s">
+      <c r="P3" s="425" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="415" t="s">
+      <c r="R3" s="435" t="s">
         <v>216</v>
       </c>
     </row>
@@ -15519,14 +15519,14 @@
       <c r="D4" s="18">
         <v>44507</v>
       </c>
-      <c r="E4" s="358" t="s">
+      <c r="E4" s="402" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="359"/>
-      <c r="H4" s="360" t="s">
+      <c r="F4" s="403"/>
+      <c r="H4" s="404" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="361"/>
+      <c r="I4" s="405"/>
       <c r="J4" s="19"/>
       <c r="K4" s="166"/>
       <c r="L4" s="20"/>
@@ -15536,15 +15536,15 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="395"/>
+      <c r="P4" s="426"/>
       <c r="Q4" s="325" t="s">
         <v>217</v>
       </c>
-      <c r="R4" s="416"/>
-      <c r="W4" s="404" t="s">
+      <c r="R4" s="436"/>
+      <c r="W4" s="408" t="s">
         <v>124</v>
       </c>
-      <c r="X4" s="404"/>
+      <c r="X4" s="408"/>
       <c r="Y4" s="227"/>
     </row>
     <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -15605,8 +15605,8 @@
       <c r="S5" s="327" t="s">
         <v>213</v>
       </c>
-      <c r="W5" s="404"/>
-      <c r="X5" s="404"/>
+      <c r="W5" s="408"/>
+      <c r="X5" s="408"/>
       <c r="Y5" s="233"/>
     </row>
     <row r="6" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16363,7 +16363,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="147"/>
-      <c r="W19" s="408">
+      <c r="W19" s="412">
         <f t="shared" ref="W19" si="3">SUM(W6:W18)</f>
         <v>0</v>
       </c>
@@ -16415,7 +16415,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="147"/>
-      <c r="W20" s="409"/>
+      <c r="W20" s="413"/>
       <c r="X20" s="269"/>
       <c r="Y20" s="233"/>
     </row>
@@ -16464,8 +16464,8 @@
         <v>0</v>
       </c>
       <c r="S21" s="147"/>
-      <c r="W21" s="410"/>
-      <c r="X21" s="410"/>
+      <c r="W21" s="414"/>
+      <c r="X21" s="414"/>
       <c r="Y21" s="233"/>
       <c r="Z21" s="128"/>
     </row>
@@ -16566,8 +16566,8 @@
         <v>0</v>
       </c>
       <c r="S23" s="147"/>
-      <c r="W23" s="411"/>
-      <c r="X23" s="411"/>
+      <c r="W23" s="415"/>
+      <c r="X23" s="415"/>
       <c r="Y23" s="233"/>
       <c r="Z23" s="128"/>
     </row>
@@ -16618,8 +16618,8 @@
         <v>0</v>
       </c>
       <c r="S24" s="147"/>
-      <c r="W24" s="411"/>
-      <c r="X24" s="411"/>
+      <c r="W24" s="415"/>
+      <c r="X24" s="415"/>
       <c r="Y24" s="233"/>
       <c r="Z24" s="128"/>
     </row>
@@ -16665,8 +16665,8 @@
       <c r="R25" s="322">
         <v>0</v>
       </c>
-      <c r="W25" s="412"/>
-      <c r="X25" s="412"/>
+      <c r="W25" s="416"/>
+      <c r="X25" s="416"/>
       <c r="Y25" s="233"/>
       <c r="Z25" s="128"/>
     </row>
@@ -16714,8 +16714,8 @@
       <c r="R26" s="322">
         <v>0</v>
       </c>
-      <c r="W26" s="412"/>
-      <c r="X26" s="412"/>
+      <c r="W26" s="416"/>
+      <c r="X26" s="416"/>
       <c r="Y26" s="233"/>
       <c r="Z26" s="128"/>
     </row>
@@ -16775,9 +16775,9 @@
       <c r="V27" t="s">
         <v>240</v>
       </c>
-      <c r="W27" s="405"/>
-      <c r="X27" s="406"/>
-      <c r="Y27" s="407"/>
+      <c r="W27" s="409"/>
+      <c r="X27" s="410"/>
+      <c r="Y27" s="411"/>
       <c r="Z27" s="128"/>
     </row>
     <row r="28" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -16831,9 +16831,9 @@
       <c r="V28" t="s">
         <v>240</v>
       </c>
-      <c r="W28" s="406"/>
-      <c r="X28" s="406"/>
-      <c r="Y28" s="407"/>
+      <c r="W28" s="410"/>
+      <c r="X28" s="410"/>
+      <c r="Y28" s="411"/>
       <c r="Z28" s="128"/>
     </row>
     <row r="29" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -17054,7 +17054,7 @@
         <v>245</v>
       </c>
       <c r="L33" s="66">
-        <v>18250.560000000001</v>
+        <v>18251.11</v>
       </c>
       <c r="M33" s="32">
         <v>0</v>
@@ -17140,11 +17140,11 @@
       <c r="J36" s="267"/>
       <c r="K36" s="250"/>
       <c r="L36" s="44"/>
-      <c r="M36" s="396">
+      <c r="M36" s="427">
         <f t="shared" ref="M36" si="4">SUM(M5:M35)</f>
         <v>1054774.3</v>
       </c>
-      <c r="N36" s="398">
+      <c r="N36" s="429">
         <f t="shared" ref="N36" si="5">SUM(N5:N35)</f>
         <v>936398</v>
       </c>
@@ -17152,7 +17152,7 @@
       <c r="P36" s="278">
         <v>0</v>
       </c>
-      <c r="Q36" s="400">
+      <c r="Q36" s="431">
         <f t="shared" ref="Q36" si="6">SUM(Q5:Q35)</f>
         <v>-37279.94</v>
       </c>
@@ -17171,13 +17171,13 @@
       <c r="J37" s="60"/>
       <c r="K37" s="41"/>
       <c r="L37" s="61"/>
-      <c r="M37" s="397"/>
-      <c r="N37" s="399"/>
+      <c r="M37" s="428"/>
+      <c r="N37" s="430"/>
       <c r="O37" s="277"/>
       <c r="P37" s="278">
         <v>0</v>
       </c>
-      <c r="Q37" s="401"/>
+      <c r="Q37" s="432"/>
     </row>
     <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
@@ -17433,7 +17433,7 @@
       </c>
       <c r="L50" s="95">
         <f>SUM(L5:L49)</f>
-        <v>59637.7</v>
+        <v>59638.25</v>
       </c>
       <c r="M50" s="96"/>
       <c r="N50" s="96"/>
@@ -17451,57 +17451,57 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="373" t="s">
+      <c r="H52" s="382" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="374"/>
+      <c r="I52" s="383"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="375">
+      <c r="K52" s="384">
         <f>I50+L50</f>
-        <v>90750.2</v>
-      </c>
-      <c r="L52" s="402"/>
+        <v>90750.75</v>
+      </c>
+      <c r="L52" s="417"/>
       <c r="M52" s="273"/>
       <c r="N52" s="273"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="13"/>
     </row>
     <row r="53" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="379" t="s">
+      <c r="D53" s="388" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="379"/>
+      <c r="E53" s="388"/>
       <c r="F53" s="315">
         <f>F50-K52-C50</f>
-        <v>1957966.6799999997</v>
+        <v>1957966.13</v>
       </c>
       <c r="I53" s="102"/>
       <c r="J53" s="103"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="403" t="s">
+      <c r="D54" s="418" t="s">
         <v>95</v>
       </c>
-      <c r="E54" s="403"/>
+      <c r="E54" s="418"/>
       <c r="F54" s="111">
         <v>-1567070.66</v>
       </c>
-      <c r="I54" s="380" t="s">
+      <c r="I54" s="389" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="381"/>
-      <c r="K54" s="382">
+      <c r="J54" s="390"/>
+      <c r="K54" s="391">
         <f>F56+F57+F58</f>
-        <v>167161.2799999998</v>
-      </c>
-      <c r="L54" s="382"/>
-      <c r="M54" s="388" t="s">
+        <v>921303.96</v>
+      </c>
+      <c r="L54" s="391"/>
+      <c r="M54" s="419" t="s">
         <v>211</v>
       </c>
-      <c r="N54" s="389"/>
-      <c r="O54" s="389"/>
-      <c r="P54" s="389"/>
-      <c r="Q54" s="390"/>
+      <c r="N54" s="420"/>
+      <c r="O54" s="420"/>
+      <c r="P54" s="420"/>
+      <c r="Q54" s="421"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="316" t="s">
@@ -17515,11 +17515,11 @@
       <c r="J55" s="106"/>
       <c r="K55" s="178"/>
       <c r="L55" s="107"/>
-      <c r="M55" s="391"/>
-      <c r="N55" s="392"/>
-      <c r="O55" s="392"/>
-      <c r="P55" s="392"/>
-      <c r="Q55" s="393"/>
+      <c r="M55" s="422"/>
+      <c r="N55" s="423"/>
+      <c r="O55" s="423"/>
+      <c r="P55" s="423"/>
+      <c r="Q55" s="424"/>
     </row>
     <row r="56" spans="1:17" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C56" s="4" t="s">
@@ -17530,18 +17530,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-199208.7200000002</v>
+        <v>-199209.27000000002</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="384">
+      <c r="K56" s="393">
         <f>-C4</f>
         <v>-567389.35</v>
       </c>
-      <c r="L56" s="385"/>
+      <c r="L56" s="394"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -17558,22 +17558,22 @@
       <c r="C58" s="112">
         <v>44563</v>
       </c>
-      <c r="D58" s="362" t="s">
+      <c r="D58" s="371" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="363"/>
+      <c r="E58" s="372"/>
       <c r="F58" s="113">
-        <v>0</v>
-      </c>
-      <c r="I58" s="364" t="s">
+        <v>754143.23</v>
+      </c>
+      <c r="I58" s="373" t="s">
         <v>198</v>
       </c>
-      <c r="J58" s="365"/>
-      <c r="K58" s="366">
+      <c r="J58" s="374"/>
+      <c r="K58" s="375">
         <f>K54+K56</f>
-        <v>-400228.07000000018</v>
-      </c>
-      <c r="L58" s="366"/>
+        <v>353914.61</v>
+      </c>
+      <c r="L58" s="375"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -17717,20 +17717,13 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="M54:Q55"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="W27:X28"/>
-    <mergeCell ref="Y27:Y28"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="N36:N37"/>
-    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="W4:X5"/>
@@ -17740,13 +17733,20 @@
     <mergeCell ref="W25:X25"/>
     <mergeCell ref="W26:X26"/>
     <mergeCell ref="R3:R4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="M54:Q55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="W27:X28"/>
+    <mergeCell ref="Y27:Y28"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="N36:N37"/>
+    <mergeCell ref="Q36:Q37"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17844,16 +17844,16 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="425" t="s">
+      <c r="A3" s="359" t="s">
         <v>195</v>
       </c>
-      <c r="B3" s="426" t="s">
+      <c r="B3" s="360" t="s">
         <v>266</v>
       </c>
       <c r="C3" s="96">
         <v>7068.6</v>
       </c>
-      <c r="D3" s="426" t="s">
+      <c r="D3" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E3" s="96">
@@ -17863,13 +17863,13 @@
         <f>C3-E3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="418" t="s">
+      <c r="I3" s="352" t="s">
         <v>195</v>
       </c>
-      <c r="J3" s="417">
+      <c r="J3" s="351">
         <v>7950</v>
       </c>
-      <c r="K3" s="419">
+      <c r="K3" s="353">
         <v>563.79999999999995</v>
       </c>
       <c r="L3" s="308"/>
@@ -17880,16 +17880,16 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="425" t="s">
+      <c r="A4" s="359" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="426" t="s">
+      <c r="B4" s="360" t="s">
         <v>267</v>
       </c>
       <c r="C4" s="96">
         <v>11495.4</v>
       </c>
-      <c r="D4" s="426" t="s">
+      <c r="D4" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E4" s="96">
@@ -17900,13 +17900,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="138"/>
-      <c r="I4" s="418" t="s">
+      <c r="I4" s="352" t="s">
         <v>195</v>
       </c>
-      <c r="J4" s="417">
+      <c r="J4" s="351">
         <v>7944</v>
       </c>
-      <c r="K4" s="419">
+      <c r="K4" s="353">
         <v>2032.08</v>
       </c>
       <c r="L4" s="290"/>
@@ -17917,16 +17917,16 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="425" t="s">
+      <c r="A5" s="359" t="s">
         <v>247</v>
       </c>
-      <c r="B5" s="426" t="s">
+      <c r="B5" s="360" t="s">
         <v>268</v>
       </c>
       <c r="C5" s="96">
         <v>276755.14</v>
       </c>
-      <c r="D5" s="426" t="s">
+      <c r="D5" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E5" s="96">
@@ -17936,13 +17936,13 @@
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="418" t="s">
+      <c r="I5" s="352" t="s">
         <v>195</v>
       </c>
-      <c r="J5" s="417">
+      <c r="J5" s="351">
         <v>7952</v>
       </c>
-      <c r="K5" s="419">
+      <c r="K5" s="353">
         <v>1756.48</v>
       </c>
       <c r="L5" s="290"/>
@@ -17953,16 +17953,16 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="425" t="s">
+      <c r="A6" s="359" t="s">
         <v>247</v>
       </c>
-      <c r="B6" s="426" t="s">
+      <c r="B6" s="360" t="s">
         <v>269</v>
       </c>
       <c r="C6" s="96">
         <v>62881.4</v>
       </c>
-      <c r="D6" s="426" t="s">
+      <c r="D6" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E6" s="96">
@@ -17972,13 +17972,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="418" t="s">
+      <c r="I6" s="352" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="417">
+      <c r="J6" s="351">
         <v>7951</v>
       </c>
-      <c r="K6" s="419">
+      <c r="K6" s="353">
         <v>7340.96</v>
       </c>
       <c r="L6" s="290"/>
@@ -17989,16 +17989,16 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="425" t="s">
+      <c r="A7" s="359" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="426" t="s">
+      <c r="B7" s="360" t="s">
         <v>270</v>
       </c>
       <c r="C7" s="96">
         <v>7868.1</v>
       </c>
-      <c r="D7" s="426" t="s">
+      <c r="D7" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E7" s="96">
@@ -18008,13 +18008,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="418" t="s">
+      <c r="I7" s="352" t="s">
         <v>247</v>
       </c>
-      <c r="J7" s="417">
+      <c r="J7" s="351">
         <v>7956</v>
       </c>
-      <c r="K7" s="419">
+      <c r="K7" s="353">
         <v>1744.64</v>
       </c>
       <c r="L7" s="290"/>
@@ -18025,16 +18025,16 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="425" t="s">
+      <c r="A8" s="359" t="s">
         <v>249</v>
       </c>
-      <c r="B8" s="426" t="s">
+      <c r="B8" s="360" t="s">
         <v>271</v>
       </c>
       <c r="C8" s="96">
         <v>22425</v>
       </c>
-      <c r="D8" s="426" t="s">
+      <c r="D8" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E8" s="96">
@@ -18044,13 +18044,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="418" t="s">
+      <c r="I8" s="352" t="s">
         <v>248</v>
       </c>
-      <c r="J8" s="417">
+      <c r="J8" s="351">
         <v>7961</v>
       </c>
-      <c r="K8" s="419">
+      <c r="K8" s="353">
         <v>6212.5</v>
       </c>
       <c r="L8" s="290"/>
@@ -18061,16 +18061,16 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="425" t="s">
+      <c r="A9" s="359" t="s">
         <v>250</v>
       </c>
-      <c r="B9" s="426" t="s">
+      <c r="B9" s="360" t="s">
         <v>272</v>
       </c>
       <c r="C9" s="96">
         <v>46727.4</v>
       </c>
-      <c r="D9" s="426" t="s">
+      <c r="D9" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E9" s="96">
@@ -18080,13 +18080,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="418" t="s">
+      <c r="I9" s="352" t="s">
         <v>249</v>
       </c>
-      <c r="J9" s="417">
+      <c r="J9" s="351">
         <v>7971</v>
       </c>
-      <c r="K9" s="419">
+      <c r="K9" s="353">
         <v>11903.89</v>
       </c>
       <c r="L9" s="290"/>
@@ -18097,16 +18097,16 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="425" t="s">
+      <c r="A10" s="359" t="s">
         <v>250</v>
       </c>
-      <c r="B10" s="426" t="s">
+      <c r="B10" s="360" t="s">
         <v>273</v>
       </c>
       <c r="C10" s="96">
         <v>8457.5</v>
       </c>
-      <c r="D10" s="426" t="s">
+      <c r="D10" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E10" s="96">
@@ -18117,13 +18117,13 @@
         <v>0</v>
       </c>
       <c r="G10" s="138"/>
-      <c r="I10" s="418" t="s">
+      <c r="I10" s="352" t="s">
         <v>249</v>
       </c>
-      <c r="J10" s="417">
+      <c r="J10" s="351">
         <v>7972</v>
       </c>
-      <c r="K10" s="419">
+      <c r="K10" s="353">
         <v>36560.6</v>
       </c>
       <c r="L10" s="290"/>
@@ -18134,16 +18134,16 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="425" t="s">
+      <c r="A11" s="359" t="s">
         <v>251</v>
       </c>
-      <c r="B11" s="426" t="s">
+      <c r="B11" s="360" t="s">
         <v>274</v>
       </c>
       <c r="C11" s="96">
         <v>112011.05</v>
       </c>
-      <c r="D11" s="426" t="s">
+      <c r="D11" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E11" s="96">
@@ -18153,13 +18153,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="418" t="s">
+      <c r="I11" s="352" t="s">
         <v>250</v>
       </c>
-      <c r="J11" s="417">
+      <c r="J11" s="351">
         <v>7975</v>
       </c>
-      <c r="K11" s="419">
+      <c r="K11" s="353">
         <v>3349.24</v>
       </c>
       <c r="L11" s="290"/>
@@ -18170,16 +18170,16 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="425" t="s">
+      <c r="A12" s="359" t="s">
         <v>275</v>
       </c>
-      <c r="B12" s="426" t="s">
+      <c r="B12" s="360" t="s">
         <v>276</v>
       </c>
       <c r="C12" s="96">
         <v>5206.45</v>
       </c>
-      <c r="D12" s="426" t="s">
+      <c r="D12" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E12" s="96">
@@ -18189,13 +18189,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="418" t="s">
+      <c r="I12" s="352" t="s">
         <v>250</v>
       </c>
-      <c r="J12" s="417">
+      <c r="J12" s="351">
         <v>7979</v>
       </c>
-      <c r="K12" s="419">
+      <c r="K12" s="353">
         <v>2755.76</v>
       </c>
       <c r="L12" s="290"/>
@@ -18206,16 +18206,16 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="425" t="s">
+      <c r="A13" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B13" s="426" t="s">
+      <c r="B13" s="360" t="s">
         <v>277</v>
       </c>
       <c r="C13" s="96">
         <v>38821.5</v>
       </c>
-      <c r="D13" s="426" t="s">
+      <c r="D13" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E13" s="96">
@@ -18225,13 +18225,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="418" t="s">
+      <c r="I13" s="352" t="s">
         <v>251</v>
       </c>
-      <c r="J13" s="417">
+      <c r="J13" s="351">
         <v>7984</v>
       </c>
-      <c r="K13" s="419">
+      <c r="K13" s="353">
         <v>19135.14</v>
       </c>
       <c r="L13" s="290"/>
@@ -18242,16 +18242,16 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="425" t="s">
+      <c r="A14" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B14" s="426" t="s">
+      <c r="B14" s="360" t="s">
         <v>278</v>
       </c>
       <c r="C14" s="96">
         <v>14425.6</v>
       </c>
-      <c r="D14" s="426" t="s">
+      <c r="D14" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E14" s="96">
@@ -18261,13 +18261,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="418" t="s">
+      <c r="I14" s="352" t="s">
         <v>252</v>
       </c>
-      <c r="J14" s="417">
+      <c r="J14" s="351">
         <v>7996</v>
       </c>
-      <c r="K14" s="419">
+      <c r="K14" s="353">
         <v>4500.16</v>
       </c>
       <c r="L14" s="290"/>
@@ -18278,16 +18278,16 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="425" t="s">
+      <c r="A15" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B15" s="426" t="s">
+      <c r="B15" s="360" t="s">
         <v>279</v>
       </c>
       <c r="C15" s="96">
         <v>9421.7000000000007</v>
       </c>
-      <c r="D15" s="426" t="s">
+      <c r="D15" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E15" s="96">
@@ -18297,13 +18297,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="418" t="s">
+      <c r="I15" s="352" t="s">
         <v>252</v>
       </c>
-      <c r="J15" s="417">
+      <c r="J15" s="351">
         <v>8002</v>
       </c>
-      <c r="K15" s="419">
+      <c r="K15" s="353">
         <v>7744</v>
       </c>
       <c r="L15" s="290"/>
@@ -18314,16 +18314,16 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="425" t="s">
+      <c r="A16" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B16" s="426" t="s">
+      <c r="B16" s="360" t="s">
         <v>280</v>
       </c>
       <c r="C16" s="96">
         <v>9069.5</v>
       </c>
-      <c r="D16" s="426" t="s">
+      <c r="D16" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E16" s="96">
@@ -18333,13 +18333,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="418" t="s">
+      <c r="I16" s="352" t="s">
         <v>253</v>
       </c>
-      <c r="J16" s="417">
+      <c r="J16" s="351">
         <v>8009</v>
       </c>
-      <c r="K16" s="419">
+      <c r="K16" s="353">
         <v>933.1</v>
       </c>
       <c r="L16" s="290"/>
@@ -18350,16 +18350,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="425" t="s">
+      <c r="A17" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B17" s="426" t="s">
+      <c r="B17" s="360" t="s">
         <v>281</v>
       </c>
       <c r="C17" s="96">
         <v>60</v>
       </c>
-      <c r="D17" s="426" t="s">
+      <c r="D17" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E17" s="96">
@@ -18369,13 +18369,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="418" t="s">
+      <c r="I17" s="352" t="s">
         <v>253</v>
       </c>
-      <c r="J17" s="417">
+      <c r="J17" s="351">
         <v>8011</v>
       </c>
-      <c r="K17" s="419">
+      <c r="K17" s="353">
         <v>2610</v>
       </c>
       <c r="L17" s="290"/>
@@ -18386,16 +18386,16 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="425" t="s">
+      <c r="A18" s="359" t="s">
         <v>252</v>
       </c>
-      <c r="B18" s="426" t="s">
+      <c r="B18" s="360" t="s">
         <v>282</v>
       </c>
       <c r="C18" s="96">
         <v>16107.5</v>
       </c>
-      <c r="D18" s="426" t="s">
+      <c r="D18" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E18" s="96">
@@ -18405,13 +18405,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="418" t="s">
+      <c r="I18" s="352" t="s">
         <v>254</v>
       </c>
-      <c r="J18" s="417">
+      <c r="J18" s="351">
         <v>8019</v>
       </c>
-      <c r="K18" s="419">
+      <c r="K18" s="353">
         <v>3554.2</v>
       </c>
       <c r="L18" s="290"/>
@@ -18422,16 +18422,16 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="425" t="s">
+      <c r="A19" s="359" t="s">
         <v>253</v>
       </c>
-      <c r="B19" s="426" t="s">
+      <c r="B19" s="360" t="s">
         <v>283</v>
       </c>
       <c r="C19" s="96">
         <v>45709</v>
       </c>
-      <c r="D19" s="426" t="s">
+      <c r="D19" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E19" s="96">
@@ -18441,13 +18441,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="418" t="s">
+      <c r="I19" s="352" t="s">
         <v>254</v>
       </c>
-      <c r="J19" s="417">
+      <c r="J19" s="351">
         <v>8024</v>
       </c>
-      <c r="K19" s="419">
+      <c r="K19" s="353">
         <v>92636.2</v>
       </c>
       <c r="L19" s="290"/>
@@ -18458,16 +18458,16 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="425" t="s">
+      <c r="A20" s="359" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="426" t="s">
+      <c r="B20" s="360" t="s">
         <v>284</v>
       </c>
       <c r="C20" s="96">
         <v>0</v>
       </c>
-      <c r="D20" s="426" t="s">
+      <c r="D20" s="360" t="s">
         <v>310</v>
       </c>
       <c r="E20" s="96">
@@ -18477,13 +18477,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="418" t="s">
+      <c r="I20" s="352" t="s">
         <v>255</v>
       </c>
-      <c r="J20" s="417">
+      <c r="J20" s="351">
         <v>8027</v>
       </c>
-      <c r="K20" s="419">
+      <c r="K20" s="353">
         <v>9327.4</v>
       </c>
       <c r="L20" s="290"/>
@@ -18494,16 +18494,16 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="425" t="s">
+      <c r="A21" s="359" t="s">
         <v>254</v>
       </c>
-      <c r="B21" s="426" t="s">
+      <c r="B21" s="360" t="s">
         <v>285</v>
       </c>
       <c r="C21" s="96">
         <v>58310.5</v>
       </c>
-      <c r="D21" s="426" t="s">
+      <c r="D21" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E21" s="96">
@@ -18513,13 +18513,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="418" t="s">
+      <c r="I21" s="352" t="s">
         <v>255</v>
       </c>
-      <c r="J21" s="417">
+      <c r="J21" s="351">
         <v>8028</v>
       </c>
-      <c r="K21" s="419">
+      <c r="K21" s="353">
         <v>428.16</v>
       </c>
       <c r="L21" s="290"/>
@@ -18530,16 +18530,16 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="425" t="s">
+      <c r="A22" s="359" t="s">
         <v>254</v>
       </c>
-      <c r="B22" s="426" t="s">
+      <c r="B22" s="360" t="s">
         <v>286</v>
       </c>
       <c r="C22" s="96">
         <v>2844.3</v>
       </c>
-      <c r="D22" s="426" t="s">
+      <c r="D22" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E22" s="96">
@@ -18550,13 +18550,13 @@
         <v>0</v>
       </c>
       <c r="G22" s="138"/>
-      <c r="I22" s="418" t="s">
+      <c r="I22" s="352" t="s">
         <v>256</v>
       </c>
-      <c r="J22" s="417">
+      <c r="J22" s="351">
         <v>8044</v>
       </c>
-      <c r="K22" s="419">
+      <c r="K22" s="353">
         <v>2709.6</v>
       </c>
       <c r="L22" s="290"/>
@@ -18567,16 +18567,16 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="425" t="s">
+      <c r="A23" s="359" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="426" t="s">
+      <c r="B23" s="360" t="s">
         <v>287</v>
       </c>
       <c r="C23" s="96">
         <v>60433.2</v>
       </c>
-      <c r="D23" s="426" t="s">
+      <c r="D23" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E23" s="96">
@@ -18586,13 +18586,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="418" t="s">
+      <c r="I23" s="352" t="s">
         <v>257</v>
       </c>
-      <c r="J23" s="417">
+      <c r="J23" s="351">
         <v>8050</v>
       </c>
-      <c r="K23" s="419">
+      <c r="K23" s="353">
         <v>1768.48</v>
       </c>
       <c r="L23" s="290"/>
@@ -18603,16 +18603,16 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="425" t="s">
+      <c r="A24" s="359" t="s">
         <v>256</v>
       </c>
-      <c r="B24" s="426" t="s">
+      <c r="B24" s="360" t="s">
         <v>288</v>
       </c>
       <c r="C24" s="96">
         <v>78786.3</v>
       </c>
-      <c r="D24" s="426" t="s">
+      <c r="D24" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E24" s="96">
@@ -18622,13 +18622,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="418" t="s">
+      <c r="I24" s="352" t="s">
         <v>257</v>
       </c>
-      <c r="J24" s="417">
+      <c r="J24" s="351">
         <v>8056</v>
       </c>
-      <c r="K24" s="419">
+      <c r="K24" s="353">
         <v>45385.8</v>
       </c>
       <c r="L24" s="290"/>
@@ -18639,16 +18639,16 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="425" t="s">
+      <c r="A25" s="359" t="s">
         <v>257</v>
       </c>
-      <c r="B25" s="426" t="s">
+      <c r="B25" s="360" t="s">
         <v>289</v>
       </c>
       <c r="C25" s="96">
         <v>36160.1</v>
       </c>
-      <c r="D25" s="426" t="s">
+      <c r="D25" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E25" s="96">
@@ -18658,13 +18658,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="418" t="s">
+      <c r="I25" s="352" t="s">
         <v>258</v>
       </c>
-      <c r="J25" s="417">
+      <c r="J25" s="351">
         <v>8065</v>
       </c>
-      <c r="K25" s="419">
+      <c r="K25" s="353">
         <v>6545.88</v>
       </c>
       <c r="L25" s="290"/>
@@ -18675,16 +18675,16 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="425" t="s">
+      <c r="A26" s="359" t="s">
         <v>257</v>
       </c>
-      <c r="B26" s="426" t="s">
+      <c r="B26" s="360" t="s">
         <v>290</v>
       </c>
       <c r="C26" s="96">
         <v>2104.4</v>
       </c>
-      <c r="D26" s="426" t="s">
+      <c r="D26" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E26" s="96">
@@ -18694,13 +18694,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="418" t="s">
+      <c r="I26" s="352" t="s">
         <v>258</v>
       </c>
-      <c r="J26" s="417">
+      <c r="J26" s="351">
         <v>8073</v>
       </c>
-      <c r="K26" s="419">
+      <c r="K26" s="353">
         <v>7998.1</v>
       </c>
       <c r="L26" s="290"/>
@@ -18711,16 +18711,16 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="425" t="s">
+      <c r="A27" s="359" t="s">
         <v>258</v>
       </c>
-      <c r="B27" s="426" t="s">
+      <c r="B27" s="360" t="s">
         <v>291</v>
       </c>
       <c r="C27" s="96">
         <v>634.5</v>
       </c>
-      <c r="D27" s="426" t="s">
+      <c r="D27" s="360" t="s">
         <v>258</v>
       </c>
       <c r="E27" s="96">
@@ -18730,13 +18730,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="418" t="s">
+      <c r="I27" s="352" t="s">
         <v>259</v>
       </c>
-      <c r="J27" s="417">
+      <c r="J27" s="351">
         <v>8080</v>
       </c>
-      <c r="K27" s="419">
+      <c r="K27" s="353">
         <v>887.52</v>
       </c>
       <c r="L27" s="290"/>
@@ -18747,16 +18747,16 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="425" t="s">
+      <c r="A28" s="359" t="s">
         <v>258</v>
       </c>
-      <c r="B28" s="426" t="s">
+      <c r="B28" s="360" t="s">
         <v>292</v>
       </c>
       <c r="C28" s="96">
         <v>47894.06</v>
       </c>
-      <c r="D28" s="426" t="s">
+      <c r="D28" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E28" s="96">
@@ -18766,13 +18766,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="418" t="s">
+      <c r="I28" s="352" t="s">
         <v>259</v>
       </c>
-      <c r="J28" s="417">
+      <c r="J28" s="351">
         <v>8083</v>
       </c>
-      <c r="K28" s="419">
+      <c r="K28" s="353">
         <v>571.6</v>
       </c>
       <c r="L28" s="290"/>
@@ -18783,16 +18783,16 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="425" t="s">
+      <c r="A29" s="359" t="s">
         <v>259</v>
       </c>
-      <c r="B29" s="426" t="s">
+      <c r="B29" s="360" t="s">
         <v>293</v>
       </c>
       <c r="C29" s="96">
         <v>48036.26</v>
       </c>
-      <c r="D29" s="426" t="s">
+      <c r="D29" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E29" s="96">
@@ -18802,13 +18802,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="418" t="s">
+      <c r="I29" s="352" t="s">
         <v>259</v>
       </c>
-      <c r="J29" s="417">
+      <c r="J29" s="351">
         <v>8090</v>
       </c>
-      <c r="K29" s="419">
+      <c r="K29" s="353">
         <v>23079</v>
       </c>
       <c r="L29" s="290"/>
@@ -18819,16 +18819,16 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="425" t="s">
+      <c r="A30" s="359" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="426" t="s">
+      <c r="B30" s="360" t="s">
         <v>294</v>
       </c>
       <c r="C30" s="96">
         <v>61444</v>
       </c>
-      <c r="D30" s="426" t="s">
+      <c r="D30" s="360" t="s">
         <v>306</v>
       </c>
       <c r="E30" s="96">
@@ -18839,13 +18839,13 @@
         <v>0</v>
       </c>
       <c r="G30" s="138"/>
-      <c r="I30" s="418" t="s">
+      <c r="I30" s="352" t="s">
         <v>260</v>
       </c>
-      <c r="J30" s="417">
+      <c r="J30" s="351">
         <v>8095</v>
       </c>
-      <c r="K30" s="419">
+      <c r="K30" s="353">
         <v>0</v>
       </c>
       <c r="L30" s="290"/>
@@ -18856,16 +18856,16 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="425" t="s">
+      <c r="A31" s="359" t="s">
         <v>260</v>
       </c>
-      <c r="B31" s="426" t="s">
+      <c r="B31" s="360" t="s">
         <v>295</v>
       </c>
       <c r="C31" s="96">
         <v>134636</v>
       </c>
-      <c r="D31" s="426" t="s">
+      <c r="D31" s="360" t="s">
         <v>311</v>
       </c>
       <c r="E31" s="96">
@@ -18875,13 +18875,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="418" t="s">
+      <c r="I31" s="352" t="s">
         <v>260</v>
       </c>
-      <c r="J31" s="417">
+      <c r="J31" s="351">
         <v>8097</v>
       </c>
-      <c r="K31" s="419">
+      <c r="K31" s="353">
         <v>288</v>
       </c>
       <c r="L31" s="290"/>
@@ -18892,16 +18892,16 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="425" t="s">
+      <c r="A32" s="359" t="s">
         <v>260</v>
       </c>
-      <c r="B32" s="426" t="s">
+      <c r="B32" s="360" t="s">
         <v>296</v>
       </c>
       <c r="C32" s="96">
         <v>2496</v>
       </c>
-      <c r="D32" s="426" t="s">
+      <c r="D32" s="360" t="s">
         <v>311</v>
       </c>
       <c r="E32" s="96">
@@ -18911,13 +18911,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="418" t="s">
+      <c r="I32" s="352" t="s">
         <v>260</v>
       </c>
-      <c r="J32" s="417">
+      <c r="J32" s="351">
         <v>8099</v>
       </c>
-      <c r="K32" s="419">
+      <c r="K32" s="353">
         <v>0</v>
       </c>
       <c r="L32" s="290"/>
@@ -18928,16 +18928,16 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="425" t="s">
+      <c r="A33" s="359" t="s">
         <v>260</v>
       </c>
-      <c r="B33" s="426" t="s">
+      <c r="B33" s="360" t="s">
         <v>297</v>
       </c>
       <c r="C33" s="96">
         <v>1835.32</v>
       </c>
-      <c r="D33" s="426" t="s">
+      <c r="D33" s="360" t="s">
         <v>311</v>
       </c>
       <c r="E33" s="96">
@@ -18947,13 +18947,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="418" t="s">
+      <c r="I33" s="352" t="s">
         <v>260</v>
       </c>
-      <c r="J33" s="417">
+      <c r="J33" s="351">
         <v>8102</v>
       </c>
-      <c r="K33" s="419">
+      <c r="K33" s="353">
         <v>16973.12</v>
       </c>
       <c r="L33" s="290"/>
@@ -18964,16 +18964,16 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="425" t="s">
+      <c r="A34" s="359" t="s">
         <v>261</v>
       </c>
-      <c r="B34" s="426" t="s">
+      <c r="B34" s="360" t="s">
         <v>298</v>
       </c>
       <c r="C34" s="96">
         <v>37820</v>
       </c>
-      <c r="D34" s="426" t="s">
+      <c r="D34" s="360" t="s">
         <v>311</v>
       </c>
       <c r="E34" s="96">
@@ -18983,13 +18983,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I34" s="418" t="s">
+      <c r="I34" s="352" t="s">
         <v>261</v>
       </c>
-      <c r="J34" s="417">
+      <c r="J34" s="351">
         <v>8104</v>
       </c>
-      <c r="K34" s="419">
+      <c r="K34" s="353">
         <v>614.24</v>
       </c>
       <c r="L34" s="290"/>
@@ -19000,16 +19000,16 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="425" t="s">
+      <c r="A35" s="359" t="s">
         <v>261</v>
       </c>
-      <c r="B35" s="426" t="s">
+      <c r="B35" s="360" t="s">
         <v>299</v>
       </c>
       <c r="C35" s="96">
         <v>20355.400000000001</v>
       </c>
-      <c r="D35" s="426" t="s">
+      <c r="D35" s="360" t="s">
         <v>311</v>
       </c>
       <c r="E35" s="96">
@@ -19019,13 +19019,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I35" s="418" t="s">
+      <c r="I35" s="352" t="s">
         <v>261</v>
       </c>
-      <c r="J35" s="417">
+      <c r="J35" s="351">
         <v>8105</v>
       </c>
-      <c r="K35" s="419">
+      <c r="K35" s="353">
         <v>216</v>
       </c>
       <c r="L35" s="290"/>
@@ -19036,10 +19036,10 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="425" t="s">
+      <c r="A36" s="359" t="s">
         <v>300</v>
       </c>
-      <c r="B36" s="426" t="s">
+      <c r="B36" s="360" t="s">
         <v>301</v>
       </c>
       <c r="C36" s="96">
@@ -19051,13 +19051,13 @@
         <f t="shared" si="0"/>
         <v>37968.800000000003</v>
       </c>
-      <c r="I36" s="418" t="s">
+      <c r="I36" s="352" t="s">
         <v>261</v>
       </c>
-      <c r="J36" s="417">
+      <c r="J36" s="351">
         <v>8110</v>
       </c>
-      <c r="K36" s="419">
+      <c r="K36" s="353">
         <v>0</v>
       </c>
       <c r="L36" s="290"/>
@@ -19068,10 +19068,10 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="425" t="s">
+      <c r="A37" s="359" t="s">
         <v>262</v>
       </c>
-      <c r="B37" s="426" t="s">
+      <c r="B37" s="360" t="s">
         <v>302</v>
       </c>
       <c r="C37" s="96">
@@ -19083,27 +19083,27 @@
         <f t="shared" si="0"/>
         <v>76339.399999999994</v>
       </c>
-      <c r="I37" s="429" t="s">
+      <c r="I37" s="363" t="s">
         <v>261</v>
       </c>
-      <c r="J37" s="430">
+      <c r="J37" s="364">
         <v>8114</v>
       </c>
-      <c r="K37" s="431">
+      <c r="K37" s="365">
         <v>78024.399999999994</v>
       </c>
-      <c r="L37" s="432"/>
-      <c r="M37" s="433"/>
-      <c r="N37" s="434">
+      <c r="L37" s="366"/>
+      <c r="M37" s="367"/>
+      <c r="N37" s="368">
         <f t="shared" si="1"/>
         <v>400150.04999999993</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="425" t="s">
+      <c r="A38" s="359" t="s">
         <v>262</v>
       </c>
-      <c r="B38" s="426" t="s">
+      <c r="B38" s="360" t="s">
         <v>303</v>
       </c>
       <c r="C38" s="96">
@@ -19115,7 +19115,7 @@
         <f t="shared" si="0"/>
         <v>78589.399999999994</v>
       </c>
-      <c r="I38" s="435" t="s">
+      <c r="I38" s="369" t="s">
         <v>262</v>
       </c>
       <c r="J38" s="38">
@@ -19126,16 +19126,16 @@
       </c>
       <c r="L38" s="290"/>
       <c r="M38" s="69"/>
-      <c r="N38" s="436">
+      <c r="N38" s="370">
         <f t="shared" si="1"/>
         <v>407494.32999999996</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="425" t="s">
+      <c r="A39" s="359" t="s">
         <v>263</v>
       </c>
-      <c r="B39" s="426" t="s">
+      <c r="B39" s="360" t="s">
         <v>304</v>
       </c>
       <c r="C39" s="96">
@@ -19147,27 +19147,27 @@
         <f t="shared" si="0"/>
         <v>114921.78</v>
       </c>
-      <c r="I39" s="420" t="s">
+      <c r="I39" s="354" t="s">
         <v>263</v>
       </c>
-      <c r="J39" s="421">
+      <c r="J39" s="355">
         <v>8144</v>
       </c>
-      <c r="K39" s="422">
-        <v>0</v>
-      </c>
-      <c r="L39" s="423"/>
+      <c r="K39" s="356">
+        <v>0</v>
+      </c>
+      <c r="L39" s="357"/>
       <c r="M39" s="215"/>
-      <c r="N39" s="424">
+      <c r="N39" s="358">
         <f t="shared" si="1"/>
         <v>407494.32999999996</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="425" t="s">
+      <c r="A40" s="359" t="s">
         <v>263</v>
       </c>
-      <c r="B40" s="426" t="s">
+      <c r="B40" s="360" t="s">
         <v>305</v>
       </c>
       <c r="C40" s="96">
@@ -19179,27 +19179,27 @@
         <f t="shared" si="0"/>
         <v>145933.38</v>
       </c>
-      <c r="I40" s="418" t="s">
+      <c r="I40" s="352" t="s">
         <v>263</v>
       </c>
-      <c r="J40" s="417">
+      <c r="J40" s="351">
         <v>8145</v>
       </c>
-      <c r="K40" s="419">
+      <c r="K40" s="353">
         <v>2592.81</v>
       </c>
       <c r="L40" s="140"/>
       <c r="M40" s="69"/>
-      <c r="N40" s="424">
+      <c r="N40" s="358">
         <f t="shared" si="1"/>
         <v>410087.13999999996</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="425" t="s">
+      <c r="A41" s="359" t="s">
         <v>306</v>
       </c>
-      <c r="B41" s="426" t="s">
+      <c r="B41" s="360" t="s">
         <v>307</v>
       </c>
       <c r="C41" s="96">
@@ -19211,27 +19211,27 @@
         <f t="shared" si="0"/>
         <v>241209.68</v>
       </c>
-      <c r="I41" s="418" t="s">
+      <c r="I41" s="352" t="s">
         <v>263</v>
       </c>
-      <c r="J41" s="417">
+      <c r="J41" s="351">
         <v>8148</v>
       </c>
-      <c r="K41" s="419">
+      <c r="K41" s="353">
         <v>89838.6</v>
       </c>
       <c r="L41" s="140"/>
       <c r="M41" s="69"/>
-      <c r="N41" s="424">
+      <c r="N41" s="358">
         <f t="shared" si="1"/>
         <v>499925.74</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="425" t="s">
+      <c r="A42" s="359" t="s">
         <v>306</v>
       </c>
-      <c r="B42" s="426" t="s">
+      <c r="B42" s="360" t="s">
         <v>308</v>
       </c>
       <c r="C42" s="96">
@@ -19243,27 +19243,27 @@
         <f t="shared" si="0"/>
         <v>245472.08</v>
       </c>
-      <c r="I42" s="418" t="s">
+      <c r="I42" s="352" t="s">
         <v>264</v>
       </c>
-      <c r="J42" s="417">
+      <c r="J42" s="351">
         <v>8164</v>
       </c>
-      <c r="K42" s="419">
+      <c r="K42" s="353">
         <v>10475.799999999999</v>
       </c>
       <c r="L42" s="140"/>
       <c r="M42" s="69"/>
-      <c r="N42" s="424">
+      <c r="N42" s="358">
         <f t="shared" si="1"/>
         <v>510401.54</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="425" t="s">
+      <c r="A43" s="359" t="s">
         <v>264</v>
       </c>
-      <c r="B43" s="426" t="s">
+      <c r="B43" s="360" t="s">
         <v>309</v>
       </c>
       <c r="C43" s="96">
@@ -19275,18 +19275,18 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I43" s="418" t="s">
+      <c r="I43" s="352" t="s">
         <v>264</v>
       </c>
-      <c r="J43" s="417">
+      <c r="J43" s="351">
         <v>8169</v>
       </c>
-      <c r="K43" s="419">
+      <c r="K43" s="353">
         <v>21719.4</v>
       </c>
       <c r="L43" s="140"/>
       <c r="M43" s="69"/>
-      <c r="N43" s="424">
+      <c r="N43" s="358">
         <f t="shared" si="1"/>
         <v>532120.93999999994</v>
       </c>
@@ -19301,18 +19301,18 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I44" s="418" t="s">
+      <c r="I44" s="352" t="s">
         <v>264</v>
       </c>
-      <c r="J44" s="417">
+      <c r="J44" s="351">
         <v>8170</v>
       </c>
-      <c r="K44" s="419">
+      <c r="K44" s="353">
         <v>57983.8</v>
       </c>
       <c r="L44" s="140"/>
       <c r="M44" s="69"/>
-      <c r="N44" s="424">
+      <c r="N44" s="358">
         <f t="shared" si="1"/>
         <v>590104.74</v>
       </c>
@@ -19567,8 +19567,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I57" s="427"/>
-      <c r="J57" s="428"/>
+      <c r="I57" s="361"/>
+      <c r="J57" s="362"/>
       <c r="K57" s="34"/>
       <c r="L57" s="147"/>
       <c r="M57" s="34"/>
@@ -19587,8 +19587,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I58" s="427"/>
-      <c r="J58" s="428"/>
+      <c r="I58" s="361"/>
+      <c r="J58" s="362"/>
       <c r="K58" s="34"/>
       <c r="L58" s="147"/>
       <c r="M58" s="34"/>
@@ -19607,8 +19607,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I59" s="427"/>
-      <c r="J59" s="428"/>
+      <c r="I59" s="361"/>
+      <c r="J59" s="362"/>
       <c r="K59" s="34"/>
       <c r="L59" s="147"/>
       <c r="M59" s="34"/>
@@ -19627,8 +19627,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I60" s="427"/>
-      <c r="J60" s="428"/>
+      <c r="I60" s="361"/>
+      <c r="J60" s="362"/>
       <c r="K60" s="34"/>
       <c r="L60" s="147"/>
       <c r="M60" s="34"/>
@@ -19647,8 +19647,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I61" s="427"/>
-      <c r="J61" s="428"/>
+      <c r="I61" s="361"/>
+      <c r="J61" s="362"/>
       <c r="K61" s="34"/>
       <c r="L61" s="147"/>
       <c r="M61" s="34"/>
@@ -19658,8 +19658,8 @@
       </c>
     </row>
     <row r="62" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="427"/>
-      <c r="B62" s="428"/>
+      <c r="A62" s="361"/>
+      <c r="B62" s="362"/>
       <c r="C62" s="34"/>
       <c r="D62" s="147"/>
       <c r="E62" s="34"/>
@@ -19667,8 +19667,8 @@
         <f t="shared" si="0"/>
         <v>278769.48</v>
       </c>
-      <c r="I62" s="427"/>
-      <c r="J62" s="428"/>
+      <c r="I62" s="361"/>
+      <c r="J62" s="362"/>
       <c r="K62" s="34"/>
       <c r="L62" s="147"/>
       <c r="M62" s="34"/>
@@ -19864,7 +19864,7 @@
       <c r="D72" s="148"/>
       <c r="E72" s="69"/>
       <c r="F72" s="137">
-        <f t="shared" ref="F57:F73" si="4">F71+C72-E72</f>
+        <f t="shared" ref="F72:F73" si="4">F71+C72-E72</f>
         <v>278769.48</v>
       </c>
       <c r="I72" s="134"/>
@@ -19929,7 +19929,7 @@
       <c r="C75" s="214"/>
       <c r="D75" s="97"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="413" t="s">
+      <c r="F75" s="433" t="s">
         <v>207</v>
       </c>
       <c r="K75" s="1"/>
@@ -19942,7 +19942,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="97"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="414"/>
+      <c r="F76" s="434"/>
       <c r="K76" s="1"/>
       <c r="L76" s="97"/>
       <c r="M76" s="3"/>

</xml_diff>